<commit_message>
fix merge xlsx (#4)
</commit_message>
<xml_diff>
--- a/csv/merge.xlsx
+++ b/csv/merge.xlsx
@@ -10663,7 +10663,7 @@
 It's a rank 3 body armor.</t>
   </si>
   <si>
-    <t>Mysterious Tower Floor 38 hint</t>
+    <t>Mysterious Tower Floor 41 hint</t>
   </si>
   <si>
     <t>&lt;pipipi_shigh&gt;「ヒヒヒ……。オイラ　なぞのツボ。
@@ -10695,7 +10695,7 @@
 angry, they can use four amazing strikes.</t>
   </si>
   <si>
-    <t>Mysterious Tower Floor 41 hint</t>
+    <t>Mysterious Tower Floor 43 hint</t>
   </si>
   <si>
     <t>&lt;pipipi_shigh&gt;「ヒヒヒ……。オイラ　なぞのツボ。
@@ -55161,4890 +55161,6 @@
       </c>
       <c r="D1049" s="2"/>
     </row>
-    <row r="1050">
-      <c r="C1050" s="9"/>
-      <c r="D1050" s="2"/>
-    </row>
-    <row r="1051">
-      <c r="A1051" s="11"/>
-      <c r="C1051" s="9"/>
-      <c r="D1051" s="2"/>
-    </row>
-    <row r="1052">
-      <c r="A1052" s="11"/>
-      <c r="C1052" s="9"/>
-      <c r="D1052" s="2"/>
-    </row>
-    <row r="1053">
-      <c r="A1053" s="11"/>
-      <c r="C1053" s="9"/>
-      <c r="D1053" s="2"/>
-    </row>
-    <row r="1054">
-      <c r="A1054" s="11"/>
-      <c r="C1054" s="9"/>
-      <c r="D1054" s="2"/>
-    </row>
-    <row r="1055">
-      <c r="A1055" s="11"/>
-      <c r="C1055" s="9"/>
-      <c r="D1055" s="2"/>
-    </row>
-    <row r="1056">
-      <c r="A1056" s="11"/>
-      <c r="C1056" s="9"/>
-      <c r="D1056" s="2"/>
-    </row>
-    <row r="1057">
-      <c r="A1057" s="11"/>
-      <c r="C1057" s="9"/>
-      <c r="D1057" s="2"/>
-    </row>
-    <row r="1058">
-      <c r="A1058" s="11"/>
-      <c r="C1058" s="9"/>
-      <c r="D1058" s="2"/>
-    </row>
-    <row r="1059">
-      <c r="A1059" s="11"/>
-      <c r="C1059" s="9"/>
-      <c r="D1059" s="2"/>
-    </row>
-    <row r="1060">
-      <c r="A1060" s="11"/>
-      <c r="C1060" s="9"/>
-      <c r="D1060" s="2"/>
-    </row>
-    <row r="1061">
-      <c r="A1061" s="11"/>
-      <c r="C1061" s="9"/>
-      <c r="D1061" s="2"/>
-    </row>
-    <row r="1062">
-      <c r="A1062" s="11"/>
-      <c r="C1062" s="9"/>
-      <c r="D1062" s="2"/>
-    </row>
-    <row r="1063">
-      <c r="A1063" s="11"/>
-      <c r="C1063" s="9"/>
-      <c r="D1063" s="2"/>
-    </row>
-    <row r="1064">
-      <c r="A1064" s="11"/>
-      <c r="C1064" s="9"/>
-      <c r="D1064" s="2"/>
-    </row>
-    <row r="1065">
-      <c r="A1065" s="11"/>
-      <c r="C1065" s="9"/>
-      <c r="D1065" s="2"/>
-    </row>
-    <row r="1066">
-      <c r="A1066" s="11"/>
-      <c r="C1066" s="9"/>
-      <c r="D1066" s="2"/>
-    </row>
-    <row r="1067">
-      <c r="A1067" s="11"/>
-      <c r="C1067" s="9"/>
-      <c r="D1067" s="2"/>
-    </row>
-    <row r="1068">
-      <c r="A1068" s="11"/>
-      <c r="C1068" s="9"/>
-      <c r="D1068" s="2"/>
-    </row>
-    <row r="1069">
-      <c r="A1069" s="11"/>
-      <c r="C1069" s="9"/>
-      <c r="D1069" s="2"/>
-    </row>
-    <row r="1070">
-      <c r="A1070" s="11"/>
-      <c r="C1070" s="9"/>
-      <c r="D1070" s="2"/>
-    </row>
-    <row r="1071">
-      <c r="A1071" s="11"/>
-      <c r="C1071" s="9"/>
-      <c r="D1071" s="2"/>
-    </row>
-    <row r="1072">
-      <c r="A1072" s="11"/>
-      <c r="C1072" s="9"/>
-      <c r="D1072" s="2"/>
-    </row>
-    <row r="1073">
-      <c r="A1073" s="11"/>
-      <c r="C1073" s="9"/>
-      <c r="D1073" s="2"/>
-    </row>
-    <row r="1074">
-      <c r="A1074" s="11"/>
-      <c r="C1074" s="9"/>
-      <c r="D1074" s="2"/>
-    </row>
-    <row r="1075">
-      <c r="A1075" s="11"/>
-      <c r="C1075" s="9"/>
-      <c r="D1075" s="2"/>
-    </row>
-    <row r="1076">
-      <c r="A1076" s="11"/>
-      <c r="C1076" s="9"/>
-      <c r="D1076" s="2"/>
-    </row>
-    <row r="1077">
-      <c r="A1077" s="11"/>
-      <c r="C1077" s="9"/>
-      <c r="D1077" s="2"/>
-    </row>
-    <row r="1078">
-      <c r="A1078" s="11"/>
-      <c r="C1078" s="9"/>
-      <c r="D1078" s="2"/>
-    </row>
-    <row r="1079">
-      <c r="A1079" s="11"/>
-      <c r="C1079" s="9"/>
-      <c r="D1079" s="2"/>
-    </row>
-    <row r="1080">
-      <c r="A1080" s="11"/>
-      <c r="C1080" s="9"/>
-      <c r="D1080" s="2"/>
-    </row>
-    <row r="1081">
-      <c r="A1081" s="11"/>
-      <c r="C1081" s="9"/>
-      <c r="D1081" s="2"/>
-    </row>
-    <row r="1082">
-      <c r="A1082" s="11"/>
-      <c r="C1082" s="9"/>
-      <c r="D1082" s="2"/>
-    </row>
-    <row r="1083">
-      <c r="A1083" s="11"/>
-      <c r="C1083" s="9"/>
-      <c r="D1083" s="2"/>
-    </row>
-    <row r="1084">
-      <c r="A1084" s="11"/>
-      <c r="C1084" s="9"/>
-      <c r="D1084" s="2"/>
-    </row>
-    <row r="1085">
-      <c r="A1085" s="11"/>
-      <c r="C1085" s="9"/>
-      <c r="D1085" s="2"/>
-    </row>
-    <row r="1086">
-      <c r="A1086" s="11"/>
-      <c r="C1086" s="9"/>
-      <c r="D1086" s="2"/>
-    </row>
-    <row r="1087">
-      <c r="A1087" s="11"/>
-      <c r="C1087" s="9"/>
-      <c r="D1087" s="2"/>
-    </row>
-    <row r="1088">
-      <c r="A1088" s="11"/>
-      <c r="C1088" s="9"/>
-      <c r="D1088" s="2"/>
-    </row>
-    <row r="1089">
-      <c r="A1089" s="11"/>
-      <c r="C1089" s="9"/>
-      <c r="D1089" s="2"/>
-    </row>
-    <row r="1090">
-      <c r="A1090" s="11"/>
-      <c r="C1090" s="9"/>
-      <c r="D1090" s="2"/>
-    </row>
-    <row r="1091">
-      <c r="A1091" s="11"/>
-      <c r="C1091" s="9"/>
-      <c r="D1091" s="2"/>
-    </row>
-    <row r="1092">
-      <c r="A1092" s="11"/>
-      <c r="C1092" s="9"/>
-      <c r="D1092" s="2"/>
-    </row>
-    <row r="1093">
-      <c r="A1093" s="11"/>
-      <c r="C1093" s="9"/>
-      <c r="D1093" s="2"/>
-    </row>
-    <row r="1094">
-      <c r="A1094" s="11"/>
-      <c r="C1094" s="9"/>
-      <c r="D1094" s="2"/>
-    </row>
-    <row r="1095">
-      <c r="A1095" s="11"/>
-      <c r="C1095" s="9"/>
-      <c r="D1095" s="2"/>
-    </row>
-    <row r="1096">
-      <c r="A1096" s="11"/>
-      <c r="C1096" s="9"/>
-      <c r="D1096" s="2"/>
-    </row>
-    <row r="1097">
-      <c r="A1097" s="11"/>
-      <c r="C1097" s="9"/>
-      <c r="D1097" s="2"/>
-    </row>
-    <row r="1098">
-      <c r="A1098" s="11"/>
-      <c r="C1098" s="9"/>
-      <c r="D1098" s="2"/>
-    </row>
-    <row r="1099">
-      <c r="A1099" s="11"/>
-      <c r="C1099" s="9"/>
-      <c r="D1099" s="2"/>
-    </row>
-    <row r="1100">
-      <c r="A1100" s="11"/>
-      <c r="C1100" s="9"/>
-      <c r="D1100" s="2"/>
-    </row>
-    <row r="1101">
-      <c r="A1101" s="11"/>
-      <c r="C1101" s="9"/>
-      <c r="D1101" s="2"/>
-    </row>
-    <row r="1102">
-      <c r="A1102" s="11"/>
-      <c r="C1102" s="9"/>
-      <c r="D1102" s="2"/>
-    </row>
-    <row r="1103">
-      <c r="A1103" s="11"/>
-      <c r="C1103" s="9"/>
-      <c r="D1103" s="2"/>
-    </row>
-    <row r="1104">
-      <c r="A1104" s="11"/>
-      <c r="C1104" s="9"/>
-      <c r="D1104" s="2"/>
-    </row>
-    <row r="1105">
-      <c r="A1105" s="11"/>
-      <c r="C1105" s="9"/>
-      <c r="D1105" s="2"/>
-    </row>
-    <row r="1106">
-      <c r="A1106" s="11"/>
-      <c r="C1106" s="9"/>
-      <c r="D1106" s="2"/>
-    </row>
-    <row r="1107">
-      <c r="A1107" s="11"/>
-      <c r="C1107" s="9"/>
-      <c r="D1107" s="2"/>
-    </row>
-    <row r="1108">
-      <c r="A1108" s="11"/>
-      <c r="C1108" s="9"/>
-      <c r="D1108" s="2"/>
-    </row>
-    <row r="1109">
-      <c r="A1109" s="11"/>
-      <c r="C1109" s="9"/>
-      <c r="D1109" s="2"/>
-    </row>
-    <row r="1110">
-      <c r="A1110" s="11"/>
-      <c r="C1110" s="9"/>
-      <c r="D1110" s="2"/>
-    </row>
-    <row r="1111">
-      <c r="A1111" s="11"/>
-      <c r="C1111" s="9"/>
-      <c r="D1111" s="2"/>
-    </row>
-    <row r="1112">
-      <c r="A1112" s="11"/>
-      <c r="C1112" s="9"/>
-      <c r="D1112" s="2"/>
-    </row>
-    <row r="1113">
-      <c r="A1113" s="11"/>
-      <c r="C1113" s="9"/>
-      <c r="D1113" s="2"/>
-    </row>
-    <row r="1114">
-      <c r="A1114" s="11"/>
-      <c r="C1114" s="9"/>
-      <c r="D1114" s="2"/>
-    </row>
-    <row r="1115">
-      <c r="A1115" s="11"/>
-      <c r="C1115" s="9"/>
-      <c r="D1115" s="2"/>
-    </row>
-    <row r="1116">
-      <c r="A1116" s="11"/>
-      <c r="C1116" s="9"/>
-      <c r="D1116" s="2"/>
-    </row>
-    <row r="1117">
-      <c r="A1117" s="11"/>
-      <c r="C1117" s="9"/>
-      <c r="D1117" s="2"/>
-    </row>
-    <row r="1118">
-      <c r="A1118" s="11"/>
-      <c r="C1118" s="9"/>
-      <c r="D1118" s="2"/>
-    </row>
-    <row r="1119">
-      <c r="A1119" s="11"/>
-      <c r="C1119" s="9"/>
-      <c r="D1119" s="2"/>
-    </row>
-    <row r="1120">
-      <c r="A1120" s="11"/>
-      <c r="C1120" s="9"/>
-      <c r="D1120" s="2"/>
-    </row>
-    <row r="1121">
-      <c r="A1121" s="11"/>
-      <c r="C1121" s="9"/>
-      <c r="D1121" s="2"/>
-    </row>
-    <row r="1122">
-      <c r="A1122" s="11"/>
-      <c r="C1122" s="9"/>
-      <c r="D1122" s="2"/>
-    </row>
-    <row r="1123">
-      <c r="A1123" s="11"/>
-      <c r="C1123" s="9"/>
-      <c r="D1123" s="2"/>
-    </row>
-    <row r="1124">
-      <c r="A1124" s="11"/>
-      <c r="C1124" s="9"/>
-      <c r="D1124" s="2"/>
-    </row>
-    <row r="1125">
-      <c r="A1125" s="11"/>
-      <c r="C1125" s="9"/>
-      <c r="D1125" s="2"/>
-    </row>
-    <row r="1126">
-      <c r="A1126" s="11"/>
-      <c r="C1126" s="9"/>
-      <c r="D1126" s="2"/>
-    </row>
-    <row r="1127">
-      <c r="A1127" s="11"/>
-      <c r="C1127" s="9"/>
-      <c r="D1127" s="2"/>
-    </row>
-    <row r="1128">
-      <c r="A1128" s="11"/>
-      <c r="C1128" s="9"/>
-      <c r="D1128" s="2"/>
-    </row>
-    <row r="1129">
-      <c r="A1129" s="11"/>
-      <c r="C1129" s="9"/>
-      <c r="D1129" s="2"/>
-    </row>
-    <row r="1130">
-      <c r="A1130" s="11"/>
-      <c r="C1130" s="9"/>
-      <c r="D1130" s="2"/>
-    </row>
-    <row r="1131">
-      <c r="A1131" s="11"/>
-      <c r="C1131" s="9"/>
-      <c r="D1131" s="2"/>
-    </row>
-    <row r="1132">
-      <c r="A1132" s="11"/>
-      <c r="C1132" s="9"/>
-      <c r="D1132" s="2"/>
-    </row>
-    <row r="1133">
-      <c r="A1133" s="11"/>
-      <c r="C1133" s="9"/>
-      <c r="D1133" s="2"/>
-    </row>
-    <row r="1134">
-      <c r="A1134" s="11"/>
-      <c r="C1134" s="9"/>
-      <c r="D1134" s="2"/>
-    </row>
-    <row r="1135">
-      <c r="A1135" s="11"/>
-      <c r="C1135" s="9"/>
-      <c r="D1135" s="2"/>
-    </row>
-    <row r="1136">
-      <c r="A1136" s="11"/>
-      <c r="C1136" s="9"/>
-      <c r="D1136" s="2"/>
-    </row>
-    <row r="1137">
-      <c r="A1137" s="11"/>
-      <c r="C1137" s="9"/>
-      <c r="D1137" s="2"/>
-    </row>
-    <row r="1138">
-      <c r="A1138" s="11"/>
-      <c r="C1138" s="9"/>
-      <c r="D1138" s="2"/>
-    </row>
-    <row r="1139">
-      <c r="A1139" s="11"/>
-      <c r="C1139" s="9"/>
-      <c r="D1139" s="2"/>
-    </row>
-    <row r="1140">
-      <c r="A1140" s="11"/>
-      <c r="C1140" s="9"/>
-      <c r="D1140" s="2"/>
-    </row>
-    <row r="1141">
-      <c r="A1141" s="11"/>
-      <c r="C1141" s="9"/>
-      <c r="D1141" s="2"/>
-    </row>
-    <row r="1142">
-      <c r="A1142" s="11"/>
-      <c r="C1142" s="9"/>
-      <c r="D1142" s="2"/>
-    </row>
-    <row r="1143">
-      <c r="A1143" s="11"/>
-      <c r="C1143" s="9"/>
-      <c r="D1143" s="2"/>
-    </row>
-    <row r="1144">
-      <c r="A1144" s="11"/>
-      <c r="C1144" s="9"/>
-      <c r="D1144" s="2"/>
-    </row>
-    <row r="1145">
-      <c r="A1145" s="11"/>
-      <c r="C1145" s="9"/>
-      <c r="D1145" s="2"/>
-    </row>
-    <row r="1146">
-      <c r="A1146" s="11"/>
-      <c r="C1146" s="9"/>
-      <c r="D1146" s="2"/>
-    </row>
-    <row r="1147">
-      <c r="A1147" s="11"/>
-      <c r="C1147" s="9"/>
-      <c r="D1147" s="2"/>
-    </row>
-    <row r="1148">
-      <c r="A1148" s="11"/>
-      <c r="C1148" s="9"/>
-      <c r="D1148" s="2"/>
-    </row>
-    <row r="1149">
-      <c r="A1149" s="11"/>
-      <c r="C1149" s="9"/>
-      <c r="D1149" s="2"/>
-    </row>
-    <row r="1150">
-      <c r="A1150" s="11"/>
-      <c r="C1150" s="9"/>
-      <c r="D1150" s="2"/>
-    </row>
-    <row r="1151">
-      <c r="A1151" s="11"/>
-      <c r="C1151" s="9"/>
-      <c r="D1151" s="2"/>
-    </row>
-    <row r="1152">
-      <c r="A1152" s="11"/>
-      <c r="C1152" s="9"/>
-      <c r="D1152" s="2"/>
-    </row>
-    <row r="1153">
-      <c r="A1153" s="11"/>
-      <c r="C1153" s="9"/>
-      <c r="D1153" s="2"/>
-    </row>
-    <row r="1154">
-      <c r="A1154" s="11"/>
-      <c r="C1154" s="9"/>
-      <c r="D1154" s="2"/>
-    </row>
-    <row r="1155">
-      <c r="A1155" s="11"/>
-      <c r="C1155" s="9"/>
-      <c r="D1155" s="2"/>
-    </row>
-    <row r="1156">
-      <c r="A1156" s="11"/>
-      <c r="C1156" s="9"/>
-      <c r="D1156" s="2"/>
-    </row>
-    <row r="1157">
-      <c r="A1157" s="11"/>
-      <c r="C1157" s="9"/>
-      <c r="D1157" s="2"/>
-    </row>
-    <row r="1158">
-      <c r="A1158" s="11"/>
-      <c r="C1158" s="9"/>
-      <c r="D1158" s="2"/>
-    </row>
-    <row r="1159">
-      <c r="A1159" s="11"/>
-      <c r="C1159" s="9"/>
-      <c r="D1159" s="2"/>
-    </row>
-    <row r="1160">
-      <c r="A1160" s="11"/>
-      <c r="C1160" s="9"/>
-      <c r="D1160" s="2"/>
-    </row>
-    <row r="1161">
-      <c r="A1161" s="11"/>
-      <c r="C1161" s="9"/>
-      <c r="D1161" s="2"/>
-    </row>
-    <row r="1162">
-      <c r="A1162" s="11"/>
-      <c r="C1162" s="9"/>
-      <c r="D1162" s="2"/>
-    </row>
-    <row r="1163">
-      <c r="A1163" s="11"/>
-      <c r="C1163" s="9"/>
-      <c r="D1163" s="2"/>
-    </row>
-    <row r="1164">
-      <c r="A1164" s="11"/>
-      <c r="C1164" s="9"/>
-      <c r="D1164" s="2"/>
-    </row>
-    <row r="1165">
-      <c r="A1165" s="11"/>
-      <c r="C1165" s="9"/>
-      <c r="D1165" s="2"/>
-    </row>
-    <row r="1166">
-      <c r="A1166" s="11"/>
-      <c r="C1166" s="9"/>
-      <c r="D1166" s="2"/>
-    </row>
-    <row r="1167">
-      <c r="A1167" s="11"/>
-      <c r="C1167" s="9"/>
-      <c r="D1167" s="2"/>
-    </row>
-    <row r="1168">
-      <c r="A1168" s="11"/>
-      <c r="C1168" s="9"/>
-      <c r="D1168" s="2"/>
-    </row>
-    <row r="1169">
-      <c r="A1169" s="11"/>
-      <c r="C1169" s="9"/>
-      <c r="D1169" s="2"/>
-    </row>
-    <row r="1170">
-      <c r="A1170" s="11"/>
-      <c r="C1170" s="9"/>
-      <c r="D1170" s="2"/>
-    </row>
-    <row r="1171">
-      <c r="A1171" s="11"/>
-      <c r="C1171" s="9"/>
-      <c r="D1171" s="2"/>
-    </row>
-    <row r="1172">
-      <c r="A1172" s="11"/>
-      <c r="C1172" s="9"/>
-      <c r="D1172" s="2"/>
-    </row>
-    <row r="1173">
-      <c r="A1173" s="11"/>
-      <c r="C1173" s="9"/>
-      <c r="D1173" s="2"/>
-    </row>
-    <row r="1174">
-      <c r="A1174" s="11"/>
-      <c r="C1174" s="9"/>
-      <c r="D1174" s="2"/>
-    </row>
-    <row r="1175">
-      <c r="A1175" s="11"/>
-      <c r="C1175" s="9"/>
-      <c r="D1175" s="2"/>
-    </row>
-    <row r="1176">
-      <c r="A1176" s="11"/>
-      <c r="C1176" s="9"/>
-      <c r="D1176" s="2"/>
-    </row>
-    <row r="1177">
-      <c r="A1177" s="11"/>
-      <c r="C1177" s="9"/>
-      <c r="D1177" s="2"/>
-    </row>
-    <row r="1178">
-      <c r="A1178" s="11"/>
-      <c r="C1178" s="9"/>
-      <c r="D1178" s="2"/>
-    </row>
-    <row r="1179">
-      <c r="A1179" s="11"/>
-      <c r="C1179" s="9"/>
-      <c r="D1179" s="2"/>
-    </row>
-    <row r="1180">
-      <c r="A1180" s="11"/>
-      <c r="C1180" s="9"/>
-      <c r="D1180" s="2"/>
-    </row>
-    <row r="1181">
-      <c r="A1181" s="11"/>
-      <c r="C1181" s="9"/>
-      <c r="D1181" s="2"/>
-    </row>
-    <row r="1182">
-      <c r="A1182" s="11"/>
-      <c r="C1182" s="9"/>
-      <c r="D1182" s="2"/>
-    </row>
-    <row r="1183">
-      <c r="A1183" s="11"/>
-      <c r="C1183" s="9"/>
-      <c r="D1183" s="2"/>
-    </row>
-    <row r="1184">
-      <c r="A1184" s="11"/>
-      <c r="C1184" s="9"/>
-      <c r="D1184" s="2"/>
-    </row>
-    <row r="1185">
-      <c r="A1185" s="11"/>
-      <c r="C1185" s="9"/>
-      <c r="D1185" s="2"/>
-    </row>
-    <row r="1186">
-      <c r="A1186" s="11"/>
-      <c r="C1186" s="9"/>
-      <c r="D1186" s="2"/>
-    </row>
-    <row r="1187">
-      <c r="A1187" s="11"/>
-      <c r="C1187" s="9"/>
-      <c r="D1187" s="2"/>
-    </row>
-    <row r="1188">
-      <c r="A1188" s="11"/>
-      <c r="C1188" s="9"/>
-      <c r="D1188" s="2"/>
-    </row>
-    <row r="1189">
-      <c r="A1189" s="11"/>
-      <c r="C1189" s="9"/>
-      <c r="D1189" s="2"/>
-    </row>
-    <row r="1190">
-      <c r="A1190" s="11"/>
-      <c r="C1190" s="9"/>
-      <c r="D1190" s="2"/>
-    </row>
-    <row r="1191">
-      <c r="A1191" s="11"/>
-      <c r="C1191" s="9"/>
-      <c r="D1191" s="2"/>
-    </row>
-    <row r="1192">
-      <c r="A1192" s="11"/>
-      <c r="C1192" s="9"/>
-      <c r="D1192" s="2"/>
-    </row>
-    <row r="1193">
-      <c r="A1193" s="11"/>
-      <c r="C1193" s="9"/>
-      <c r="D1193" s="2"/>
-    </row>
-    <row r="1194">
-      <c r="A1194" s="11"/>
-      <c r="C1194" s="9"/>
-      <c r="D1194" s="2"/>
-    </row>
-    <row r="1195">
-      <c r="A1195" s="11"/>
-      <c r="C1195" s="9"/>
-      <c r="D1195" s="2"/>
-    </row>
-    <row r="1196">
-      <c r="A1196" s="11"/>
-      <c r="C1196" s="9"/>
-      <c r="D1196" s="2"/>
-    </row>
-    <row r="1197">
-      <c r="A1197" s="11"/>
-      <c r="C1197" s="9"/>
-      <c r="D1197" s="2"/>
-    </row>
-    <row r="1198">
-      <c r="A1198" s="11"/>
-      <c r="C1198" s="9"/>
-      <c r="D1198" s="2"/>
-    </row>
-    <row r="1199">
-      <c r="A1199" s="11"/>
-      <c r="C1199" s="9"/>
-      <c r="D1199" s="2"/>
-    </row>
-    <row r="1200">
-      <c r="A1200" s="11"/>
-      <c r="C1200" s="9"/>
-      <c r="D1200" s="2"/>
-    </row>
-    <row r="1201">
-      <c r="A1201" s="11"/>
-      <c r="C1201" s="9"/>
-      <c r="D1201" s="2"/>
-    </row>
-    <row r="1202">
-      <c r="A1202" s="11"/>
-      <c r="C1202" s="9"/>
-      <c r="D1202" s="2"/>
-    </row>
-    <row r="1203">
-      <c r="A1203" s="11"/>
-      <c r="C1203" s="9"/>
-      <c r="D1203" s="2"/>
-    </row>
-    <row r="1204">
-      <c r="A1204" s="11"/>
-      <c r="C1204" s="9"/>
-      <c r="D1204" s="2"/>
-    </row>
-    <row r="1205">
-      <c r="A1205" s="11"/>
-      <c r="C1205" s="9"/>
-      <c r="D1205" s="2"/>
-    </row>
-    <row r="1206">
-      <c r="A1206" s="11"/>
-      <c r="C1206" s="9"/>
-      <c r="D1206" s="2"/>
-    </row>
-    <row r="1207">
-      <c r="A1207" s="11"/>
-      <c r="C1207" s="9"/>
-      <c r="D1207" s="2"/>
-    </row>
-    <row r="1208">
-      <c r="A1208" s="11"/>
-      <c r="C1208" s="9"/>
-      <c r="D1208" s="2"/>
-    </row>
-    <row r="1209">
-      <c r="A1209" s="11"/>
-      <c r="C1209" s="9"/>
-      <c r="D1209" s="2"/>
-    </row>
-    <row r="1210">
-      <c r="A1210" s="11"/>
-      <c r="C1210" s="9"/>
-      <c r="D1210" s="2"/>
-    </row>
-    <row r="1211">
-      <c r="A1211" s="11"/>
-      <c r="C1211" s="9"/>
-      <c r="D1211" s="2"/>
-    </row>
-    <row r="1212">
-      <c r="A1212" s="11"/>
-      <c r="C1212" s="9"/>
-      <c r="D1212" s="2"/>
-    </row>
-    <row r="1213">
-      <c r="A1213" s="11"/>
-      <c r="C1213" s="9"/>
-      <c r="D1213" s="2"/>
-    </row>
-    <row r="1214">
-      <c r="A1214" s="11"/>
-      <c r="C1214" s="9"/>
-      <c r="D1214" s="2"/>
-    </row>
-    <row r="1215">
-      <c r="A1215" s="11"/>
-      <c r="C1215" s="9"/>
-      <c r="D1215" s="2"/>
-    </row>
-    <row r="1216">
-      <c r="A1216" s="11"/>
-      <c r="C1216" s="9"/>
-      <c r="D1216" s="2"/>
-    </row>
-    <row r="1217">
-      <c r="A1217" s="11"/>
-      <c r="C1217" s="9"/>
-      <c r="D1217" s="2"/>
-    </row>
-    <row r="1218">
-      <c r="A1218" s="11"/>
-      <c r="C1218" s="9"/>
-      <c r="D1218" s="2"/>
-    </row>
-    <row r="1219">
-      <c r="A1219" s="11"/>
-      <c r="C1219" s="9"/>
-      <c r="D1219" s="2"/>
-    </row>
-    <row r="1220">
-      <c r="A1220" s="11"/>
-      <c r="C1220" s="9"/>
-      <c r="D1220" s="2"/>
-    </row>
-    <row r="1221">
-      <c r="A1221" s="11"/>
-      <c r="C1221" s="9"/>
-      <c r="D1221" s="2"/>
-    </row>
-    <row r="1222">
-      <c r="A1222" s="11"/>
-      <c r="C1222" s="9"/>
-      <c r="D1222" s="2"/>
-    </row>
-    <row r="1223">
-      <c r="A1223" s="11"/>
-      <c r="C1223" s="9"/>
-      <c r="D1223" s="2"/>
-    </row>
-    <row r="1224">
-      <c r="A1224" s="11"/>
-      <c r="C1224" s="9"/>
-      <c r="D1224" s="2"/>
-    </row>
-    <row r="1225">
-      <c r="A1225" s="11"/>
-      <c r="C1225" s="9"/>
-      <c r="D1225" s="2"/>
-    </row>
-    <row r="1226">
-      <c r="A1226" s="11"/>
-      <c r="C1226" s="9"/>
-      <c r="D1226" s="2"/>
-    </row>
-    <row r="1227">
-      <c r="A1227" s="11"/>
-      <c r="C1227" s="9"/>
-      <c r="D1227" s="2"/>
-    </row>
-    <row r="1228">
-      <c r="A1228" s="11"/>
-      <c r="C1228" s="9"/>
-      <c r="D1228" s="2"/>
-    </row>
-    <row r="1229">
-      <c r="A1229" s="11"/>
-      <c r="C1229" s="9"/>
-      <c r="D1229" s="2"/>
-    </row>
-    <row r="1230">
-      <c r="A1230" s="11"/>
-      <c r="C1230" s="9"/>
-      <c r="D1230" s="2"/>
-    </row>
-    <row r="1231">
-      <c r="A1231" s="11"/>
-      <c r="C1231" s="9"/>
-      <c r="D1231" s="2"/>
-    </row>
-    <row r="1232">
-      <c r="A1232" s="11"/>
-      <c r="C1232" s="9"/>
-      <c r="D1232" s="2"/>
-    </row>
-    <row r="1233">
-      <c r="A1233" s="11"/>
-      <c r="C1233" s="9"/>
-      <c r="D1233" s="2"/>
-    </row>
-    <row r="1234">
-      <c r="A1234" s="11"/>
-      <c r="C1234" s="9"/>
-      <c r="D1234" s="2"/>
-    </row>
-    <row r="1235">
-      <c r="A1235" s="11"/>
-      <c r="C1235" s="9"/>
-      <c r="D1235" s="2"/>
-    </row>
-    <row r="1236">
-      <c r="A1236" s="11"/>
-      <c r="C1236" s="9"/>
-      <c r="D1236" s="2"/>
-    </row>
-    <row r="1237">
-      <c r="A1237" s="11"/>
-      <c r="C1237" s="9"/>
-      <c r="D1237" s="2"/>
-    </row>
-    <row r="1238">
-      <c r="A1238" s="11"/>
-      <c r="C1238" s="9"/>
-      <c r="D1238" s="2"/>
-    </row>
-    <row r="1239">
-      <c r="A1239" s="11"/>
-      <c r="C1239" s="9"/>
-      <c r="D1239" s="2"/>
-    </row>
-    <row r="1240">
-      <c r="A1240" s="11"/>
-      <c r="C1240" s="9"/>
-      <c r="D1240" s="2"/>
-    </row>
-    <row r="1241">
-      <c r="A1241" s="11"/>
-      <c r="C1241" s="9"/>
-      <c r="D1241" s="2"/>
-    </row>
-    <row r="1242">
-      <c r="A1242" s="11"/>
-      <c r="C1242" s="9"/>
-      <c r="D1242" s="2"/>
-    </row>
-    <row r="1243">
-      <c r="A1243" s="11"/>
-      <c r="C1243" s="9"/>
-      <c r="D1243" s="2"/>
-    </row>
-    <row r="1244">
-      <c r="A1244" s="11"/>
-      <c r="C1244" s="9"/>
-      <c r="D1244" s="2"/>
-    </row>
-    <row r="1245">
-      <c r="A1245" s="11"/>
-      <c r="C1245" s="9"/>
-      <c r="D1245" s="2"/>
-    </row>
-    <row r="1246">
-      <c r="A1246" s="11"/>
-      <c r="C1246" s="9"/>
-      <c r="D1246" s="2"/>
-    </row>
-    <row r="1247">
-      <c r="A1247" s="11"/>
-      <c r="C1247" s="9"/>
-      <c r="D1247" s="2"/>
-    </row>
-    <row r="1248">
-      <c r="A1248" s="11"/>
-      <c r="C1248" s="9"/>
-      <c r="D1248" s="2"/>
-    </row>
-    <row r="1249">
-      <c r="A1249" s="11"/>
-      <c r="C1249" s="9"/>
-      <c r="D1249" s="2"/>
-    </row>
-    <row r="1250">
-      <c r="A1250" s="11"/>
-      <c r="C1250" s="9"/>
-      <c r="D1250" s="2"/>
-    </row>
-    <row r="1251">
-      <c r="A1251" s="11"/>
-      <c r="C1251" s="9"/>
-      <c r="D1251" s="2"/>
-    </row>
-    <row r="1252">
-      <c r="A1252" s="11"/>
-      <c r="C1252" s="9"/>
-      <c r="D1252" s="2"/>
-    </row>
-    <row r="1253">
-      <c r="A1253" s="11"/>
-      <c r="C1253" s="9"/>
-      <c r="D1253" s="2"/>
-    </row>
-    <row r="1254">
-      <c r="A1254" s="11"/>
-      <c r="C1254" s="9"/>
-      <c r="D1254" s="2"/>
-    </row>
-    <row r="1255">
-      <c r="A1255" s="11"/>
-      <c r="C1255" s="9"/>
-      <c r="D1255" s="2"/>
-    </row>
-    <row r="1256">
-      <c r="A1256" s="11"/>
-      <c r="C1256" s="9"/>
-      <c r="D1256" s="2"/>
-    </row>
-    <row r="1257">
-      <c r="A1257" s="11"/>
-      <c r="C1257" s="9"/>
-      <c r="D1257" s="2"/>
-    </row>
-    <row r="1258">
-      <c r="A1258" s="11"/>
-      <c r="C1258" s="9"/>
-      <c r="D1258" s="2"/>
-    </row>
-    <row r="1259">
-      <c r="A1259" s="11"/>
-      <c r="C1259" s="9"/>
-      <c r="D1259" s="2"/>
-    </row>
-    <row r="1260">
-      <c r="A1260" s="11"/>
-      <c r="C1260" s="9"/>
-      <c r="D1260" s="2"/>
-    </row>
-    <row r="1261">
-      <c r="A1261" s="11"/>
-      <c r="C1261" s="9"/>
-      <c r="D1261" s="2"/>
-    </row>
-    <row r="1262">
-      <c r="A1262" s="11"/>
-      <c r="C1262" s="9"/>
-      <c r="D1262" s="2"/>
-    </row>
-    <row r="1263">
-      <c r="A1263" s="11"/>
-      <c r="C1263" s="9"/>
-      <c r="D1263" s="2"/>
-    </row>
-    <row r="1264">
-      <c r="A1264" s="11"/>
-      <c r="C1264" s="9"/>
-      <c r="D1264" s="2"/>
-    </row>
-    <row r="1265">
-      <c r="A1265" s="11"/>
-      <c r="C1265" s="9"/>
-      <c r="D1265" s="2"/>
-    </row>
-    <row r="1266">
-      <c r="A1266" s="11"/>
-      <c r="C1266" s="9"/>
-      <c r="D1266" s="2"/>
-    </row>
-    <row r="1267">
-      <c r="A1267" s="11"/>
-      <c r="C1267" s="9"/>
-      <c r="D1267" s="2"/>
-    </row>
-    <row r="1268">
-      <c r="A1268" s="11"/>
-      <c r="C1268" s="9"/>
-      <c r="D1268" s="2"/>
-    </row>
-    <row r="1269">
-      <c r="A1269" s="11"/>
-      <c r="C1269" s="9"/>
-      <c r="D1269" s="2"/>
-    </row>
-    <row r="1270">
-      <c r="A1270" s="11"/>
-      <c r="C1270" s="9"/>
-      <c r="D1270" s="2"/>
-    </row>
-    <row r="1271">
-      <c r="A1271" s="11"/>
-      <c r="C1271" s="9"/>
-      <c r="D1271" s="2"/>
-    </row>
-    <row r="1272">
-      <c r="A1272" s="11"/>
-      <c r="C1272" s="9"/>
-      <c r="D1272" s="2"/>
-    </row>
-    <row r="1273">
-      <c r="A1273" s="11"/>
-      <c r="C1273" s="9"/>
-      <c r="D1273" s="2"/>
-    </row>
-    <row r="1274">
-      <c r="A1274" s="11"/>
-      <c r="C1274" s="9"/>
-      <c r="D1274" s="2"/>
-    </row>
-    <row r="1275">
-      <c r="A1275" s="11"/>
-      <c r="C1275" s="9"/>
-      <c r="D1275" s="2"/>
-    </row>
-    <row r="1276">
-      <c r="A1276" s="11"/>
-      <c r="C1276" s="9"/>
-      <c r="D1276" s="2"/>
-    </row>
-    <row r="1277">
-      <c r="A1277" s="11"/>
-      <c r="C1277" s="9"/>
-      <c r="D1277" s="2"/>
-    </row>
-    <row r="1278">
-      <c r="A1278" s="11"/>
-      <c r="C1278" s="9"/>
-      <c r="D1278" s="2"/>
-    </row>
-    <row r="1279">
-      <c r="A1279" s="11"/>
-      <c r="C1279" s="9"/>
-      <c r="D1279" s="2"/>
-    </row>
-    <row r="1280">
-      <c r="A1280" s="11"/>
-      <c r="C1280" s="9"/>
-      <c r="D1280" s="2"/>
-    </row>
-    <row r="1281">
-      <c r="A1281" s="11"/>
-      <c r="C1281" s="9"/>
-      <c r="D1281" s="2"/>
-    </row>
-    <row r="1282">
-      <c r="A1282" s="11"/>
-      <c r="C1282" s="9"/>
-      <c r="D1282" s="2"/>
-    </row>
-    <row r="1283">
-      <c r="A1283" s="11"/>
-      <c r="C1283" s="9"/>
-      <c r="D1283" s="2"/>
-    </row>
-    <row r="1284">
-      <c r="A1284" s="11"/>
-      <c r="C1284" s="9"/>
-      <c r="D1284" s="2"/>
-    </row>
-    <row r="1285">
-      <c r="A1285" s="11"/>
-      <c r="C1285" s="9"/>
-      <c r="D1285" s="2"/>
-    </row>
-    <row r="1286">
-      <c r="A1286" s="11"/>
-      <c r="C1286" s="9"/>
-      <c r="D1286" s="2"/>
-    </row>
-    <row r="1287">
-      <c r="A1287" s="11"/>
-      <c r="C1287" s="9"/>
-      <c r="D1287" s="2"/>
-    </row>
-    <row r="1288">
-      <c r="A1288" s="11"/>
-      <c r="C1288" s="9"/>
-      <c r="D1288" s="2"/>
-    </row>
-    <row r="1289">
-      <c r="A1289" s="11"/>
-      <c r="C1289" s="9"/>
-      <c r="D1289" s="2"/>
-    </row>
-    <row r="1290">
-      <c r="A1290" s="11"/>
-      <c r="C1290" s="9"/>
-      <c r="D1290" s="2"/>
-    </row>
-    <row r="1291">
-      <c r="A1291" s="11"/>
-      <c r="C1291" s="9"/>
-      <c r="D1291" s="2"/>
-    </row>
-    <row r="1292">
-      <c r="A1292" s="11"/>
-      <c r="C1292" s="9"/>
-      <c r="D1292" s="2"/>
-    </row>
-    <row r="1293">
-      <c r="A1293" s="11"/>
-      <c r="C1293" s="9"/>
-      <c r="D1293" s="2"/>
-    </row>
-    <row r="1294">
-      <c r="A1294" s="11"/>
-      <c r="C1294" s="9"/>
-      <c r="D1294" s="2"/>
-    </row>
-    <row r="1295">
-      <c r="A1295" s="11"/>
-      <c r="C1295" s="9"/>
-      <c r="D1295" s="2"/>
-    </row>
-    <row r="1296">
-      <c r="A1296" s="11"/>
-      <c r="C1296" s="9"/>
-      <c r="D1296" s="2"/>
-    </row>
-    <row r="1297">
-      <c r="A1297" s="11"/>
-      <c r="C1297" s="9"/>
-      <c r="D1297" s="2"/>
-    </row>
-    <row r="1298">
-      <c r="A1298" s="11"/>
-      <c r="C1298" s="9"/>
-      <c r="D1298" s="2"/>
-    </row>
-    <row r="1299">
-      <c r="A1299" s="11"/>
-      <c r="C1299" s="9"/>
-      <c r="D1299" s="2"/>
-    </row>
-    <row r="1300">
-      <c r="A1300" s="11"/>
-      <c r="C1300" s="9"/>
-      <c r="D1300" s="2"/>
-    </row>
-    <row r="1301">
-      <c r="A1301" s="11"/>
-      <c r="C1301" s="9"/>
-      <c r="D1301" s="2"/>
-    </row>
-    <row r="1302">
-      <c r="A1302" s="11"/>
-      <c r="C1302" s="9"/>
-      <c r="D1302" s="2"/>
-    </row>
-    <row r="1303">
-      <c r="A1303" s="11"/>
-      <c r="C1303" s="9"/>
-      <c r="D1303" s="2"/>
-    </row>
-    <row r="1304">
-      <c r="A1304" s="11"/>
-      <c r="C1304" s="9"/>
-      <c r="D1304" s="2"/>
-    </row>
-    <row r="1305">
-      <c r="A1305" s="11"/>
-      <c r="C1305" s="9"/>
-      <c r="D1305" s="2"/>
-    </row>
-    <row r="1306">
-      <c r="A1306" s="11"/>
-      <c r="C1306" s="9"/>
-      <c r="D1306" s="2"/>
-    </row>
-    <row r="1307">
-      <c r="A1307" s="11"/>
-      <c r="C1307" s="9"/>
-      <c r="D1307" s="2"/>
-    </row>
-    <row r="1308">
-      <c r="A1308" s="11"/>
-      <c r="C1308" s="9"/>
-      <c r="D1308" s="2"/>
-    </row>
-    <row r="1309">
-      <c r="A1309" s="11"/>
-      <c r="C1309" s="9"/>
-      <c r="D1309" s="2"/>
-    </row>
-    <row r="1310">
-      <c r="A1310" s="11"/>
-      <c r="C1310" s="9"/>
-      <c r="D1310" s="2"/>
-    </row>
-    <row r="1311">
-      <c r="A1311" s="11"/>
-      <c r="C1311" s="9"/>
-      <c r="D1311" s="2"/>
-    </row>
-    <row r="1312">
-      <c r="A1312" s="11"/>
-      <c r="C1312" s="9"/>
-      <c r="D1312" s="2"/>
-    </row>
-    <row r="1313">
-      <c r="A1313" s="11"/>
-      <c r="C1313" s="9"/>
-      <c r="D1313" s="2"/>
-    </row>
-    <row r="1314">
-      <c r="A1314" s="11"/>
-      <c r="C1314" s="9"/>
-      <c r="D1314" s="2"/>
-    </row>
-    <row r="1315">
-      <c r="A1315" s="11"/>
-      <c r="C1315" s="9"/>
-      <c r="D1315" s="2"/>
-    </row>
-    <row r="1316">
-      <c r="A1316" s="11"/>
-      <c r="C1316" s="9"/>
-      <c r="D1316" s="2"/>
-    </row>
-    <row r="1317">
-      <c r="A1317" s="11"/>
-      <c r="C1317" s="9"/>
-      <c r="D1317" s="2"/>
-    </row>
-    <row r="1318">
-      <c r="A1318" s="11"/>
-      <c r="C1318" s="9"/>
-      <c r="D1318" s="2"/>
-    </row>
-    <row r="1319">
-      <c r="A1319" s="11"/>
-      <c r="C1319" s="9"/>
-      <c r="D1319" s="2"/>
-    </row>
-    <row r="1320">
-      <c r="A1320" s="11"/>
-      <c r="C1320" s="9"/>
-      <c r="D1320" s="2"/>
-    </row>
-    <row r="1321">
-      <c r="A1321" s="11"/>
-      <c r="C1321" s="9"/>
-      <c r="D1321" s="2"/>
-    </row>
-    <row r="1322">
-      <c r="A1322" s="11"/>
-      <c r="C1322" s="9"/>
-      <c r="D1322" s="2"/>
-    </row>
-    <row r="1323">
-      <c r="A1323" s="11"/>
-      <c r="C1323" s="9"/>
-      <c r="D1323" s="2"/>
-    </row>
-    <row r="1324">
-      <c r="A1324" s="11"/>
-      <c r="C1324" s="9"/>
-      <c r="D1324" s="2"/>
-    </row>
-    <row r="1325">
-      <c r="A1325" s="11"/>
-      <c r="C1325" s="9"/>
-      <c r="D1325" s="2"/>
-    </row>
-    <row r="1326">
-      <c r="A1326" s="11"/>
-      <c r="C1326" s="9"/>
-      <c r="D1326" s="2"/>
-    </row>
-    <row r="1327">
-      <c r="A1327" s="11"/>
-      <c r="C1327" s="9"/>
-      <c r="D1327" s="2"/>
-    </row>
-    <row r="1328">
-      <c r="A1328" s="11"/>
-      <c r="C1328" s="9"/>
-      <c r="D1328" s="2"/>
-    </row>
-    <row r="1329">
-      <c r="A1329" s="11"/>
-      <c r="C1329" s="9"/>
-      <c r="D1329" s="2"/>
-    </row>
-    <row r="1330">
-      <c r="A1330" s="11"/>
-      <c r="C1330" s="9"/>
-      <c r="D1330" s="2"/>
-    </row>
-    <row r="1331">
-      <c r="A1331" s="11"/>
-      <c r="C1331" s="9"/>
-      <c r="D1331" s="2"/>
-    </row>
-    <row r="1332">
-      <c r="A1332" s="11"/>
-      <c r="C1332" s="9"/>
-      <c r="D1332" s="2"/>
-    </row>
-    <row r="1333">
-      <c r="A1333" s="11"/>
-      <c r="C1333" s="9"/>
-      <c r="D1333" s="2"/>
-    </row>
-    <row r="1334">
-      <c r="A1334" s="11"/>
-      <c r="C1334" s="9"/>
-      <c r="D1334" s="2"/>
-    </row>
-    <row r="1335">
-      <c r="A1335" s="11"/>
-      <c r="C1335" s="9"/>
-      <c r="D1335" s="2"/>
-    </row>
-    <row r="1336">
-      <c r="A1336" s="11"/>
-      <c r="C1336" s="9"/>
-      <c r="D1336" s="2"/>
-    </row>
-    <row r="1337">
-      <c r="A1337" s="11"/>
-      <c r="C1337" s="9"/>
-      <c r="D1337" s="2"/>
-    </row>
-    <row r="1338">
-      <c r="A1338" s="11"/>
-      <c r="C1338" s="9"/>
-      <c r="D1338" s="2"/>
-    </row>
-    <row r="1339">
-      <c r="A1339" s="11"/>
-      <c r="C1339" s="9"/>
-      <c r="D1339" s="2"/>
-    </row>
-    <row r="1340">
-      <c r="A1340" s="11"/>
-      <c r="C1340" s="9"/>
-      <c r="D1340" s="2"/>
-    </row>
-    <row r="1341">
-      <c r="A1341" s="11"/>
-      <c r="C1341" s="9"/>
-      <c r="D1341" s="2"/>
-    </row>
-    <row r="1342">
-      <c r="A1342" s="11"/>
-      <c r="C1342" s="9"/>
-      <c r="D1342" s="2"/>
-    </row>
-    <row r="1343">
-      <c r="A1343" s="11"/>
-      <c r="C1343" s="9"/>
-      <c r="D1343" s="2"/>
-    </row>
-    <row r="1344">
-      <c r="A1344" s="11"/>
-      <c r="C1344" s="9"/>
-      <c r="D1344" s="2"/>
-    </row>
-    <row r="1345">
-      <c r="A1345" s="11"/>
-      <c r="C1345" s="9"/>
-      <c r="D1345" s="2"/>
-    </row>
-    <row r="1346">
-      <c r="A1346" s="11"/>
-      <c r="C1346" s="9"/>
-      <c r="D1346" s="2"/>
-    </row>
-    <row r="1347">
-      <c r="A1347" s="11"/>
-      <c r="C1347" s="9"/>
-      <c r="D1347" s="2"/>
-    </row>
-    <row r="1348">
-      <c r="A1348" s="11"/>
-      <c r="C1348" s="9"/>
-      <c r="D1348" s="2"/>
-    </row>
-    <row r="1349">
-      <c r="A1349" s="11"/>
-      <c r="C1349" s="9"/>
-      <c r="D1349" s="2"/>
-    </row>
-    <row r="1350">
-      <c r="A1350" s="11"/>
-      <c r="C1350" s="9"/>
-      <c r="D1350" s="2"/>
-    </row>
-    <row r="1351">
-      <c r="A1351" s="11"/>
-      <c r="C1351" s="9"/>
-      <c r="D1351" s="2"/>
-    </row>
-    <row r="1352">
-      <c r="A1352" s="11"/>
-      <c r="C1352" s="9"/>
-      <c r="D1352" s="2"/>
-    </row>
-    <row r="1353">
-      <c r="A1353" s="11"/>
-      <c r="C1353" s="9"/>
-      <c r="D1353" s="2"/>
-    </row>
-    <row r="1354">
-      <c r="A1354" s="11"/>
-      <c r="C1354" s="9"/>
-      <c r="D1354" s="2"/>
-    </row>
-    <row r="1355">
-      <c r="A1355" s="11"/>
-      <c r="C1355" s="9"/>
-      <c r="D1355" s="2"/>
-    </row>
-    <row r="1356">
-      <c r="A1356" s="11"/>
-      <c r="C1356" s="9"/>
-      <c r="D1356" s="2"/>
-    </row>
-    <row r="1357">
-      <c r="A1357" s="11"/>
-      <c r="C1357" s="9"/>
-      <c r="D1357" s="2"/>
-    </row>
-    <row r="1358">
-      <c r="A1358" s="11"/>
-      <c r="C1358" s="9"/>
-      <c r="D1358" s="2"/>
-    </row>
-    <row r="1359">
-      <c r="A1359" s="11"/>
-      <c r="C1359" s="9"/>
-      <c r="D1359" s="2"/>
-    </row>
-    <row r="1360">
-      <c r="A1360" s="11"/>
-      <c r="C1360" s="9"/>
-      <c r="D1360" s="2"/>
-    </row>
-    <row r="1361">
-      <c r="A1361" s="11"/>
-      <c r="C1361" s="9"/>
-      <c r="D1361" s="2"/>
-    </row>
-    <row r="1362">
-      <c r="A1362" s="11"/>
-      <c r="C1362" s="9"/>
-      <c r="D1362" s="2"/>
-    </row>
-    <row r="1363">
-      <c r="A1363" s="11"/>
-      <c r="C1363" s="9"/>
-      <c r="D1363" s="2"/>
-    </row>
-    <row r="1364">
-      <c r="A1364" s="11"/>
-      <c r="C1364" s="9"/>
-      <c r="D1364" s="2"/>
-    </row>
-    <row r="1365">
-      <c r="A1365" s="11"/>
-      <c r="C1365" s="9"/>
-      <c r="D1365" s="2"/>
-    </row>
-    <row r="1366">
-      <c r="A1366" s="11"/>
-      <c r="C1366" s="9"/>
-      <c r="D1366" s="2"/>
-    </row>
-    <row r="1367">
-      <c r="A1367" s="11"/>
-      <c r="C1367" s="9"/>
-      <c r="D1367" s="2"/>
-    </row>
-    <row r="1368">
-      <c r="A1368" s="11"/>
-      <c r="C1368" s="9"/>
-      <c r="D1368" s="2"/>
-    </row>
-    <row r="1369">
-      <c r="A1369" s="11"/>
-      <c r="C1369" s="9"/>
-      <c r="D1369" s="2"/>
-    </row>
-    <row r="1370">
-      <c r="A1370" s="11"/>
-      <c r="C1370" s="9"/>
-      <c r="D1370" s="2"/>
-    </row>
-    <row r="1371">
-      <c r="A1371" s="11"/>
-      <c r="C1371" s="9"/>
-      <c r="D1371" s="2"/>
-    </row>
-    <row r="1372">
-      <c r="A1372" s="11"/>
-      <c r="C1372" s="9"/>
-      <c r="D1372" s="2"/>
-    </row>
-    <row r="1373">
-      <c r="A1373" s="11"/>
-      <c r="C1373" s="9"/>
-      <c r="D1373" s="2"/>
-    </row>
-    <row r="1374">
-      <c r="A1374" s="11"/>
-      <c r="C1374" s="9"/>
-      <c r="D1374" s="2"/>
-    </row>
-    <row r="1375">
-      <c r="A1375" s="11"/>
-      <c r="C1375" s="9"/>
-      <c r="D1375" s="2"/>
-    </row>
-    <row r="1376">
-      <c r="A1376" s="11"/>
-      <c r="C1376" s="9"/>
-      <c r="D1376" s="2"/>
-    </row>
-    <row r="1377">
-      <c r="A1377" s="11"/>
-      <c r="C1377" s="9"/>
-      <c r="D1377" s="2"/>
-    </row>
-    <row r="1378">
-      <c r="A1378" s="11"/>
-      <c r="C1378" s="9"/>
-      <c r="D1378" s="2"/>
-    </row>
-    <row r="1379">
-      <c r="A1379" s="11"/>
-      <c r="C1379" s="9"/>
-      <c r="D1379" s="2"/>
-    </row>
-    <row r="1380">
-      <c r="A1380" s="11"/>
-      <c r="C1380" s="9"/>
-      <c r="D1380" s="2"/>
-    </row>
-    <row r="1381">
-      <c r="A1381" s="11"/>
-      <c r="C1381" s="9"/>
-      <c r="D1381" s="2"/>
-    </row>
-    <row r="1382">
-      <c r="A1382" s="11"/>
-      <c r="C1382" s="9"/>
-      <c r="D1382" s="2"/>
-    </row>
-    <row r="1383">
-      <c r="A1383" s="11"/>
-      <c r="C1383" s="9"/>
-      <c r="D1383" s="2"/>
-    </row>
-    <row r="1384">
-      <c r="A1384" s="11"/>
-      <c r="C1384" s="9"/>
-      <c r="D1384" s="2"/>
-    </row>
-    <row r="1385">
-      <c r="A1385" s="11"/>
-      <c r="C1385" s="9"/>
-      <c r="D1385" s="2"/>
-    </row>
-    <row r="1386">
-      <c r="A1386" s="11"/>
-      <c r="C1386" s="9"/>
-      <c r="D1386" s="2"/>
-    </row>
-    <row r="1387">
-      <c r="A1387" s="11"/>
-      <c r="C1387" s="9"/>
-      <c r="D1387" s="2"/>
-    </row>
-    <row r="1388">
-      <c r="A1388" s="11"/>
-      <c r="C1388" s="9"/>
-      <c r="D1388" s="2"/>
-    </row>
-    <row r="1389">
-      <c r="A1389" s="11"/>
-      <c r="C1389" s="9"/>
-      <c r="D1389" s="2"/>
-    </row>
-    <row r="1390">
-      <c r="A1390" s="11"/>
-      <c r="C1390" s="9"/>
-      <c r="D1390" s="2"/>
-    </row>
-    <row r="1391">
-      <c r="A1391" s="11"/>
-      <c r="C1391" s="9"/>
-      <c r="D1391" s="2"/>
-    </row>
-    <row r="1392">
-      <c r="A1392" s="11"/>
-      <c r="C1392" s="9"/>
-      <c r="D1392" s="2"/>
-    </row>
-    <row r="1393">
-      <c r="A1393" s="11"/>
-      <c r="C1393" s="9"/>
-      <c r="D1393" s="2"/>
-    </row>
-    <row r="1394">
-      <c r="A1394" s="11"/>
-      <c r="C1394" s="9"/>
-      <c r="D1394" s="2"/>
-    </row>
-    <row r="1395">
-      <c r="A1395" s="11"/>
-      <c r="C1395" s="9"/>
-      <c r="D1395" s="2"/>
-    </row>
-    <row r="1396">
-      <c r="A1396" s="11"/>
-      <c r="C1396" s="9"/>
-      <c r="D1396" s="2"/>
-    </row>
-    <row r="1397">
-      <c r="A1397" s="11"/>
-      <c r="C1397" s="9"/>
-      <c r="D1397" s="2"/>
-    </row>
-    <row r="1398">
-      <c r="A1398" s="11"/>
-      <c r="C1398" s="9"/>
-      <c r="D1398" s="2"/>
-    </row>
-    <row r="1399">
-      <c r="A1399" s="11"/>
-      <c r="C1399" s="9"/>
-      <c r="D1399" s="2"/>
-    </row>
-    <row r="1400">
-      <c r="A1400" s="11"/>
-      <c r="C1400" s="9"/>
-      <c r="D1400" s="2"/>
-    </row>
-    <row r="1401">
-      <c r="A1401" s="11"/>
-      <c r="C1401" s="9"/>
-      <c r="D1401" s="2"/>
-    </row>
-    <row r="1402">
-      <c r="A1402" s="11"/>
-      <c r="C1402" s="9"/>
-      <c r="D1402" s="2"/>
-    </row>
-    <row r="1403">
-      <c r="A1403" s="11"/>
-      <c r="C1403" s="9"/>
-      <c r="D1403" s="2"/>
-    </row>
-    <row r="1404">
-      <c r="A1404" s="11"/>
-      <c r="C1404" s="9"/>
-      <c r="D1404" s="2"/>
-    </row>
-    <row r="1405">
-      <c r="A1405" s="11"/>
-      <c r="C1405" s="9"/>
-      <c r="D1405" s="2"/>
-    </row>
-    <row r="1406">
-      <c r="A1406" s="11"/>
-      <c r="C1406" s="9"/>
-      <c r="D1406" s="2"/>
-    </row>
-    <row r="1407">
-      <c r="A1407" s="11"/>
-      <c r="C1407" s="9"/>
-      <c r="D1407" s="2"/>
-    </row>
-    <row r="1408">
-      <c r="A1408" s="11"/>
-      <c r="C1408" s="9"/>
-      <c r="D1408" s="2"/>
-    </row>
-    <row r="1409">
-      <c r="A1409" s="11"/>
-      <c r="C1409" s="9"/>
-      <c r="D1409" s="2"/>
-    </row>
-    <row r="1410">
-      <c r="A1410" s="11"/>
-      <c r="C1410" s="9"/>
-      <c r="D1410" s="2"/>
-    </row>
-    <row r="1411">
-      <c r="A1411" s="11"/>
-      <c r="C1411" s="9"/>
-      <c r="D1411" s="2"/>
-    </row>
-    <row r="1412">
-      <c r="A1412" s="11"/>
-      <c r="C1412" s="9"/>
-      <c r="D1412" s="2"/>
-    </row>
-    <row r="1413">
-      <c r="A1413" s="11"/>
-      <c r="C1413" s="9"/>
-      <c r="D1413" s="2"/>
-    </row>
-    <row r="1414">
-      <c r="A1414" s="11"/>
-      <c r="C1414" s="9"/>
-      <c r="D1414" s="2"/>
-    </row>
-    <row r="1415">
-      <c r="A1415" s="11"/>
-      <c r="C1415" s="9"/>
-      <c r="D1415" s="2"/>
-    </row>
-    <row r="1416">
-      <c r="A1416" s="11"/>
-      <c r="C1416" s="9"/>
-      <c r="D1416" s="2"/>
-    </row>
-    <row r="1417">
-      <c r="A1417" s="11"/>
-      <c r="C1417" s="9"/>
-      <c r="D1417" s="2"/>
-    </row>
-    <row r="1418">
-      <c r="A1418" s="11"/>
-      <c r="C1418" s="9"/>
-      <c r="D1418" s="2"/>
-    </row>
-    <row r="1419">
-      <c r="A1419" s="11"/>
-      <c r="C1419" s="9"/>
-      <c r="D1419" s="2"/>
-    </row>
-    <row r="1420">
-      <c r="A1420" s="11"/>
-      <c r="C1420" s="9"/>
-      <c r="D1420" s="2"/>
-    </row>
-    <row r="1421">
-      <c r="A1421" s="11"/>
-      <c r="C1421" s="9"/>
-      <c r="D1421" s="2"/>
-    </row>
-    <row r="1422">
-      <c r="A1422" s="11"/>
-      <c r="C1422" s="9"/>
-      <c r="D1422" s="2"/>
-    </row>
-    <row r="1423">
-      <c r="A1423" s="11"/>
-      <c r="C1423" s="9"/>
-      <c r="D1423" s="2"/>
-    </row>
-    <row r="1424">
-      <c r="A1424" s="11"/>
-      <c r="C1424" s="9"/>
-      <c r="D1424" s="2"/>
-    </row>
-    <row r="1425">
-      <c r="A1425" s="11"/>
-      <c r="C1425" s="9"/>
-      <c r="D1425" s="2"/>
-    </row>
-    <row r="1426">
-      <c r="A1426" s="11"/>
-      <c r="C1426" s="9"/>
-      <c r="D1426" s="2"/>
-    </row>
-    <row r="1427">
-      <c r="A1427" s="11"/>
-      <c r="C1427" s="9"/>
-      <c r="D1427" s="2"/>
-    </row>
-    <row r="1428">
-      <c r="A1428" s="11"/>
-      <c r="C1428" s="9"/>
-      <c r="D1428" s="2"/>
-    </row>
-    <row r="1429">
-      <c r="A1429" s="11"/>
-      <c r="C1429" s="9"/>
-      <c r="D1429" s="2"/>
-    </row>
-    <row r="1430">
-      <c r="A1430" s="11"/>
-      <c r="C1430" s="9"/>
-      <c r="D1430" s="2"/>
-    </row>
-    <row r="1431">
-      <c r="A1431" s="11"/>
-      <c r="C1431" s="9"/>
-      <c r="D1431" s="2"/>
-    </row>
-    <row r="1432">
-      <c r="A1432" s="11"/>
-      <c r="C1432" s="9"/>
-      <c r="D1432" s="2"/>
-    </row>
-    <row r="1433">
-      <c r="A1433" s="11"/>
-      <c r="C1433" s="9"/>
-      <c r="D1433" s="2"/>
-    </row>
-    <row r="1434">
-      <c r="A1434" s="11"/>
-      <c r="C1434" s="9"/>
-      <c r="D1434" s="2"/>
-    </row>
-    <row r="1435">
-      <c r="A1435" s="11"/>
-      <c r="C1435" s="9"/>
-      <c r="D1435" s="2"/>
-    </row>
-    <row r="1436">
-      <c r="A1436" s="11"/>
-      <c r="C1436" s="9"/>
-      <c r="D1436" s="2"/>
-    </row>
-    <row r="1437">
-      <c r="A1437" s="11"/>
-      <c r="C1437" s="9"/>
-      <c r="D1437" s="2"/>
-    </row>
-    <row r="1438">
-      <c r="A1438" s="11"/>
-      <c r="C1438" s="9"/>
-      <c r="D1438" s="2"/>
-    </row>
-    <row r="1439">
-      <c r="A1439" s="11"/>
-      <c r="C1439" s="9"/>
-      <c r="D1439" s="2"/>
-    </row>
-    <row r="1440">
-      <c r="A1440" s="11"/>
-      <c r="C1440" s="9"/>
-      <c r="D1440" s="2"/>
-    </row>
-    <row r="1441">
-      <c r="A1441" s="11"/>
-      <c r="C1441" s="9"/>
-      <c r="D1441" s="2"/>
-    </row>
-    <row r="1442">
-      <c r="A1442" s="11"/>
-      <c r="C1442" s="9"/>
-      <c r="D1442" s="2"/>
-    </row>
-    <row r="1443">
-      <c r="A1443" s="11"/>
-      <c r="C1443" s="9"/>
-      <c r="D1443" s="2"/>
-    </row>
-    <row r="1444">
-      <c r="A1444" s="11"/>
-      <c r="C1444" s="9"/>
-      <c r="D1444" s="2"/>
-    </row>
-    <row r="1445">
-      <c r="A1445" s="11"/>
-      <c r="C1445" s="9"/>
-      <c r="D1445" s="2"/>
-    </row>
-    <row r="1446">
-      <c r="A1446" s="11"/>
-      <c r="C1446" s="9"/>
-      <c r="D1446" s="2"/>
-    </row>
-    <row r="1447">
-      <c r="A1447" s="11"/>
-      <c r="C1447" s="9"/>
-      <c r="D1447" s="2"/>
-    </row>
-    <row r="1448">
-      <c r="A1448" s="11"/>
-      <c r="C1448" s="9"/>
-      <c r="D1448" s="2"/>
-    </row>
-    <row r="1449">
-      <c r="A1449" s="11"/>
-      <c r="C1449" s="9"/>
-      <c r="D1449" s="2"/>
-    </row>
-    <row r="1450">
-      <c r="A1450" s="11"/>
-      <c r="C1450" s="9"/>
-      <c r="D1450" s="2"/>
-    </row>
-    <row r="1451">
-      <c r="A1451" s="11"/>
-      <c r="C1451" s="9"/>
-      <c r="D1451" s="2"/>
-    </row>
-    <row r="1452">
-      <c r="A1452" s="11"/>
-      <c r="C1452" s="9"/>
-      <c r="D1452" s="2"/>
-    </row>
-    <row r="1453">
-      <c r="A1453" s="11"/>
-      <c r="C1453" s="9"/>
-      <c r="D1453" s="2"/>
-    </row>
-    <row r="1454">
-      <c r="A1454" s="11"/>
-      <c r="C1454" s="9"/>
-      <c r="D1454" s="2"/>
-    </row>
-    <row r="1455">
-      <c r="A1455" s="11"/>
-      <c r="C1455" s="9"/>
-      <c r="D1455" s="2"/>
-    </row>
-    <row r="1456">
-      <c r="A1456" s="11"/>
-      <c r="C1456" s="9"/>
-      <c r="D1456" s="2"/>
-    </row>
-    <row r="1457">
-      <c r="A1457" s="11"/>
-      <c r="C1457" s="9"/>
-      <c r="D1457" s="2"/>
-    </row>
-    <row r="1458">
-      <c r="A1458" s="11"/>
-      <c r="C1458" s="9"/>
-      <c r="D1458" s="2"/>
-    </row>
-    <row r="1459">
-      <c r="A1459" s="11"/>
-      <c r="C1459" s="9"/>
-      <c r="D1459" s="2"/>
-    </row>
-    <row r="1460">
-      <c r="A1460" s="11"/>
-      <c r="C1460" s="9"/>
-      <c r="D1460" s="2"/>
-    </row>
-    <row r="1461">
-      <c r="A1461" s="11"/>
-      <c r="C1461" s="9"/>
-      <c r="D1461" s="2"/>
-    </row>
-    <row r="1462">
-      <c r="A1462" s="11"/>
-      <c r="C1462" s="9"/>
-      <c r="D1462" s="2"/>
-    </row>
-    <row r="1463">
-      <c r="A1463" s="11"/>
-      <c r="C1463" s="9"/>
-      <c r="D1463" s="2"/>
-    </row>
-    <row r="1464">
-      <c r="A1464" s="11"/>
-      <c r="C1464" s="9"/>
-      <c r="D1464" s="2"/>
-    </row>
-    <row r="1465">
-      <c r="A1465" s="11"/>
-      <c r="C1465" s="9"/>
-      <c r="D1465" s="2"/>
-    </row>
-    <row r="1466">
-      <c r="A1466" s="11"/>
-      <c r="C1466" s="9"/>
-      <c r="D1466" s="2"/>
-    </row>
-    <row r="1467">
-      <c r="A1467" s="11"/>
-      <c r="C1467" s="9"/>
-      <c r="D1467" s="2"/>
-    </row>
-    <row r="1468">
-      <c r="A1468" s="11"/>
-      <c r="C1468" s="9"/>
-      <c r="D1468" s="2"/>
-    </row>
-    <row r="1469">
-      <c r="A1469" s="11"/>
-      <c r="C1469" s="9"/>
-      <c r="D1469" s="2"/>
-    </row>
-    <row r="1470">
-      <c r="A1470" s="11"/>
-      <c r="C1470" s="9"/>
-      <c r="D1470" s="2"/>
-    </row>
-    <row r="1471">
-      <c r="A1471" s="11"/>
-      <c r="C1471" s="9"/>
-      <c r="D1471" s="2"/>
-    </row>
-    <row r="1472">
-      <c r="A1472" s="11"/>
-      <c r="C1472" s="9"/>
-      <c r="D1472" s="2"/>
-    </row>
-    <row r="1473">
-      <c r="A1473" s="11"/>
-      <c r="C1473" s="9"/>
-      <c r="D1473" s="2"/>
-    </row>
-    <row r="1474">
-      <c r="A1474" s="11"/>
-      <c r="C1474" s="9"/>
-      <c r="D1474" s="2"/>
-    </row>
-    <row r="1475">
-      <c r="A1475" s="11"/>
-      <c r="C1475" s="9"/>
-      <c r="D1475" s="2"/>
-    </row>
-    <row r="1476">
-      <c r="A1476" s="11"/>
-      <c r="C1476" s="9"/>
-      <c r="D1476" s="2"/>
-    </row>
-    <row r="1477">
-      <c r="A1477" s="11"/>
-      <c r="C1477" s="9"/>
-      <c r="D1477" s="2"/>
-    </row>
-    <row r="1478">
-      <c r="A1478" s="11"/>
-      <c r="C1478" s="9"/>
-      <c r="D1478" s="2"/>
-    </row>
-    <row r="1479">
-      <c r="A1479" s="11"/>
-      <c r="C1479" s="9"/>
-      <c r="D1479" s="2"/>
-    </row>
-    <row r="1480">
-      <c r="A1480" s="11"/>
-      <c r="C1480" s="9"/>
-      <c r="D1480" s="2"/>
-    </row>
-    <row r="1481">
-      <c r="A1481" s="11"/>
-      <c r="C1481" s="9"/>
-      <c r="D1481" s="2"/>
-    </row>
-    <row r="1482">
-      <c r="A1482" s="11"/>
-      <c r="C1482" s="9"/>
-      <c r="D1482" s="2"/>
-    </row>
-    <row r="1483">
-      <c r="A1483" s="11"/>
-      <c r="C1483" s="9"/>
-      <c r="D1483" s="2"/>
-    </row>
-    <row r="1484">
-      <c r="A1484" s="11"/>
-      <c r="C1484" s="9"/>
-      <c r="D1484" s="2"/>
-    </row>
-    <row r="1485">
-      <c r="A1485" s="11"/>
-      <c r="C1485" s="9"/>
-      <c r="D1485" s="2"/>
-    </row>
-    <row r="1486">
-      <c r="A1486" s="11"/>
-      <c r="C1486" s="9"/>
-      <c r="D1486" s="2"/>
-    </row>
-    <row r="1487">
-      <c r="A1487" s="11"/>
-      <c r="C1487" s="9"/>
-      <c r="D1487" s="2"/>
-    </row>
-    <row r="1488">
-      <c r="A1488" s="11"/>
-      <c r="C1488" s="9"/>
-      <c r="D1488" s="2"/>
-    </row>
-    <row r="1489">
-      <c r="A1489" s="11"/>
-      <c r="C1489" s="9"/>
-      <c r="D1489" s="2"/>
-    </row>
-    <row r="1490">
-      <c r="A1490" s="11"/>
-      <c r="C1490" s="9"/>
-      <c r="D1490" s="2"/>
-    </row>
-    <row r="1491">
-      <c r="A1491" s="11"/>
-      <c r="C1491" s="9"/>
-      <c r="D1491" s="2"/>
-    </row>
-    <row r="1492">
-      <c r="A1492" s="11"/>
-      <c r="C1492" s="9"/>
-      <c r="D1492" s="2"/>
-    </row>
-    <row r="1493">
-      <c r="A1493" s="11"/>
-      <c r="C1493" s="9"/>
-      <c r="D1493" s="2"/>
-    </row>
-    <row r="1494">
-      <c r="A1494" s="11"/>
-      <c r="C1494" s="9"/>
-      <c r="D1494" s="2"/>
-    </row>
-    <row r="1495">
-      <c r="A1495" s="11"/>
-      <c r="C1495" s="9"/>
-      <c r="D1495" s="2"/>
-    </row>
-    <row r="1496">
-      <c r="A1496" s="11"/>
-      <c r="C1496" s="9"/>
-      <c r="D1496" s="2"/>
-    </row>
-    <row r="1497">
-      <c r="A1497" s="11"/>
-      <c r="C1497" s="9"/>
-      <c r="D1497" s="2"/>
-    </row>
-    <row r="1498">
-      <c r="A1498" s="11"/>
-      <c r="C1498" s="9"/>
-      <c r="D1498" s="2"/>
-    </row>
-    <row r="1499">
-      <c r="A1499" s="11"/>
-      <c r="C1499" s="9"/>
-      <c r="D1499" s="2"/>
-    </row>
-    <row r="1500">
-      <c r="A1500" s="11"/>
-      <c r="C1500" s="9"/>
-      <c r="D1500" s="2"/>
-    </row>
-    <row r="1501">
-      <c r="A1501" s="11"/>
-      <c r="C1501" s="9"/>
-      <c r="D1501" s="2"/>
-    </row>
-    <row r="1502">
-      <c r="A1502" s="11"/>
-      <c r="C1502" s="9"/>
-      <c r="D1502" s="2"/>
-    </row>
-    <row r="1503">
-      <c r="A1503" s="11"/>
-      <c r="C1503" s="9"/>
-      <c r="D1503" s="2"/>
-    </row>
-    <row r="1504">
-      <c r="A1504" s="11"/>
-      <c r="C1504" s="9"/>
-      <c r="D1504" s="2"/>
-    </row>
-    <row r="1505">
-      <c r="A1505" s="11"/>
-      <c r="C1505" s="9"/>
-      <c r="D1505" s="2"/>
-    </row>
-    <row r="1506">
-      <c r="A1506" s="11"/>
-      <c r="C1506" s="9"/>
-      <c r="D1506" s="2"/>
-    </row>
-    <row r="1507">
-      <c r="A1507" s="11"/>
-      <c r="C1507" s="9"/>
-      <c r="D1507" s="2"/>
-    </row>
-    <row r="1508">
-      <c r="A1508" s="11"/>
-      <c r="C1508" s="9"/>
-      <c r="D1508" s="2"/>
-    </row>
-    <row r="1509">
-      <c r="A1509" s="11"/>
-      <c r="C1509" s="9"/>
-      <c r="D1509" s="2"/>
-    </row>
-    <row r="1510">
-      <c r="A1510" s="11"/>
-      <c r="C1510" s="9"/>
-      <c r="D1510" s="2"/>
-    </row>
-    <row r="1511">
-      <c r="A1511" s="11"/>
-      <c r="C1511" s="9"/>
-      <c r="D1511" s="2"/>
-    </row>
-    <row r="1512">
-      <c r="A1512" s="11"/>
-      <c r="C1512" s="9"/>
-      <c r="D1512" s="2"/>
-    </row>
-    <row r="1513">
-      <c r="A1513" s="11"/>
-      <c r="C1513" s="9"/>
-      <c r="D1513" s="2"/>
-    </row>
-    <row r="1514">
-      <c r="A1514" s="11"/>
-      <c r="C1514" s="9"/>
-      <c r="D1514" s="2"/>
-    </row>
-    <row r="1515">
-      <c r="A1515" s="11"/>
-      <c r="C1515" s="9"/>
-      <c r="D1515" s="2"/>
-    </row>
-    <row r="1516">
-      <c r="A1516" s="11"/>
-      <c r="C1516" s="9"/>
-      <c r="D1516" s="2"/>
-    </row>
-    <row r="1517">
-      <c r="A1517" s="11"/>
-      <c r="C1517" s="9"/>
-      <c r="D1517" s="2"/>
-    </row>
-    <row r="1518">
-      <c r="A1518" s="11"/>
-      <c r="C1518" s="9"/>
-      <c r="D1518" s="2"/>
-    </row>
-    <row r="1519">
-      <c r="A1519" s="11"/>
-      <c r="C1519" s="9"/>
-      <c r="D1519" s="2"/>
-    </row>
-    <row r="1520">
-      <c r="A1520" s="11"/>
-      <c r="C1520" s="9"/>
-      <c r="D1520" s="2"/>
-    </row>
-    <row r="1521">
-      <c r="A1521" s="11"/>
-      <c r="C1521" s="9"/>
-      <c r="D1521" s="2"/>
-    </row>
-    <row r="1522">
-      <c r="A1522" s="11"/>
-      <c r="C1522" s="9"/>
-      <c r="D1522" s="2"/>
-    </row>
-    <row r="1523">
-      <c r="A1523" s="11"/>
-      <c r="C1523" s="9"/>
-      <c r="D1523" s="2"/>
-    </row>
-    <row r="1524">
-      <c r="A1524" s="11"/>
-      <c r="C1524" s="9"/>
-      <c r="D1524" s="2"/>
-    </row>
-    <row r="1525">
-      <c r="A1525" s="11"/>
-      <c r="C1525" s="9"/>
-      <c r="D1525" s="2"/>
-    </row>
-    <row r="1526">
-      <c r="A1526" s="11"/>
-      <c r="C1526" s="9"/>
-      <c r="D1526" s="2"/>
-    </row>
-    <row r="1527">
-      <c r="A1527" s="11"/>
-      <c r="C1527" s="9"/>
-      <c r="D1527" s="2"/>
-    </row>
-    <row r="1528">
-      <c r="A1528" s="11"/>
-      <c r="C1528" s="9"/>
-      <c r="D1528" s="2"/>
-    </row>
-    <row r="1529">
-      <c r="A1529" s="11"/>
-      <c r="C1529" s="9"/>
-      <c r="D1529" s="2"/>
-    </row>
-    <row r="1530">
-      <c r="A1530" s="11"/>
-      <c r="C1530" s="9"/>
-      <c r="D1530" s="2"/>
-    </row>
-    <row r="1531">
-      <c r="A1531" s="11"/>
-      <c r="C1531" s="9"/>
-      <c r="D1531" s="2"/>
-    </row>
-    <row r="1532">
-      <c r="A1532" s="11"/>
-      <c r="C1532" s="9"/>
-      <c r="D1532" s="2"/>
-    </row>
-    <row r="1533">
-      <c r="A1533" s="11"/>
-      <c r="C1533" s="9"/>
-      <c r="D1533" s="2"/>
-    </row>
-    <row r="1534">
-      <c r="A1534" s="11"/>
-      <c r="C1534" s="9"/>
-      <c r="D1534" s="2"/>
-    </row>
-    <row r="1535">
-      <c r="A1535" s="11"/>
-      <c r="C1535" s="9"/>
-      <c r="D1535" s="2"/>
-    </row>
-    <row r="1536">
-      <c r="A1536" s="11"/>
-      <c r="C1536" s="9"/>
-      <c r="D1536" s="2"/>
-    </row>
-    <row r="1537">
-      <c r="A1537" s="11"/>
-      <c r="C1537" s="9"/>
-      <c r="D1537" s="2"/>
-    </row>
-    <row r="1538">
-      <c r="A1538" s="11"/>
-      <c r="C1538" s="9"/>
-      <c r="D1538" s="2"/>
-    </row>
-    <row r="1539">
-      <c r="A1539" s="11"/>
-      <c r="C1539" s="9"/>
-      <c r="D1539" s="2"/>
-    </row>
-    <row r="1540">
-      <c r="A1540" s="11"/>
-      <c r="C1540" s="9"/>
-      <c r="D1540" s="2"/>
-    </row>
-    <row r="1541">
-      <c r="A1541" s="11"/>
-      <c r="C1541" s="9"/>
-      <c r="D1541" s="2"/>
-    </row>
-    <row r="1542">
-      <c r="A1542" s="11"/>
-      <c r="C1542" s="9"/>
-      <c r="D1542" s="2"/>
-    </row>
-    <row r="1543">
-      <c r="A1543" s="11"/>
-      <c r="C1543" s="9"/>
-      <c r="D1543" s="2"/>
-    </row>
-    <row r="1544">
-      <c r="A1544" s="11"/>
-      <c r="C1544" s="9"/>
-      <c r="D1544" s="2"/>
-    </row>
-    <row r="1545">
-      <c r="A1545" s="11"/>
-      <c r="C1545" s="9"/>
-      <c r="D1545" s="2"/>
-    </row>
-    <row r="1546">
-      <c r="A1546" s="11"/>
-      <c r="C1546" s="9"/>
-      <c r="D1546" s="2"/>
-    </row>
-    <row r="1547">
-      <c r="A1547" s="11"/>
-      <c r="C1547" s="9"/>
-      <c r="D1547" s="2"/>
-    </row>
-    <row r="1548">
-      <c r="A1548" s="11"/>
-      <c r="C1548" s="9"/>
-      <c r="D1548" s="2"/>
-    </row>
-    <row r="1549">
-      <c r="A1549" s="11"/>
-      <c r="C1549" s="9"/>
-      <c r="D1549" s="2"/>
-    </row>
-    <row r="1550">
-      <c r="A1550" s="11"/>
-      <c r="C1550" s="9"/>
-      <c r="D1550" s="2"/>
-    </row>
-    <row r="1551">
-      <c r="A1551" s="11"/>
-      <c r="C1551" s="9"/>
-      <c r="D1551" s="2"/>
-    </row>
-    <row r="1552">
-      <c r="A1552" s="11"/>
-      <c r="C1552" s="9"/>
-      <c r="D1552" s="2"/>
-    </row>
-    <row r="1553">
-      <c r="A1553" s="11"/>
-      <c r="C1553" s="9"/>
-      <c r="D1553" s="2"/>
-    </row>
-    <row r="1554">
-      <c r="A1554" s="11"/>
-      <c r="C1554" s="9"/>
-      <c r="D1554" s="2"/>
-    </row>
-    <row r="1555">
-      <c r="A1555" s="11"/>
-      <c r="C1555" s="9"/>
-      <c r="D1555" s="2"/>
-    </row>
-    <row r="1556">
-      <c r="A1556" s="11"/>
-      <c r="C1556" s="9"/>
-      <c r="D1556" s="2"/>
-    </row>
-    <row r="1557">
-      <c r="A1557" s="11"/>
-      <c r="C1557" s="9"/>
-      <c r="D1557" s="2"/>
-    </row>
-    <row r="1558">
-      <c r="A1558" s="11"/>
-      <c r="C1558" s="9"/>
-      <c r="D1558" s="2"/>
-    </row>
-    <row r="1559">
-      <c r="A1559" s="11"/>
-      <c r="C1559" s="9"/>
-      <c r="D1559" s="2"/>
-    </row>
-    <row r="1560">
-      <c r="A1560" s="11"/>
-      <c r="C1560" s="9"/>
-      <c r="D1560" s="2"/>
-    </row>
-    <row r="1561">
-      <c r="A1561" s="11"/>
-      <c r="C1561" s="9"/>
-      <c r="D1561" s="2"/>
-    </row>
-    <row r="1562">
-      <c r="A1562" s="11"/>
-      <c r="C1562" s="9"/>
-      <c r="D1562" s="2"/>
-    </row>
-    <row r="1563">
-      <c r="A1563" s="11"/>
-      <c r="C1563" s="9"/>
-      <c r="D1563" s="2"/>
-    </row>
-    <row r="1564">
-      <c r="A1564" s="11"/>
-      <c r="C1564" s="9"/>
-      <c r="D1564" s="2"/>
-    </row>
-    <row r="1565">
-      <c r="A1565" s="11"/>
-      <c r="C1565" s="9"/>
-      <c r="D1565" s="2"/>
-    </row>
-    <row r="1566">
-      <c r="A1566" s="11"/>
-      <c r="C1566" s="9"/>
-      <c r="D1566" s="2"/>
-    </row>
-    <row r="1567">
-      <c r="A1567" s="11"/>
-      <c r="C1567" s="9"/>
-      <c r="D1567" s="2"/>
-    </row>
-    <row r="1568">
-      <c r="A1568" s="11"/>
-      <c r="C1568" s="9"/>
-      <c r="D1568" s="2"/>
-    </row>
-    <row r="1569">
-      <c r="A1569" s="11"/>
-      <c r="C1569" s="9"/>
-      <c r="D1569" s="2"/>
-    </row>
-    <row r="1570">
-      <c r="A1570" s="11"/>
-      <c r="C1570" s="9"/>
-      <c r="D1570" s="2"/>
-    </row>
-    <row r="1571">
-      <c r="A1571" s="11"/>
-      <c r="C1571" s="9"/>
-      <c r="D1571" s="2"/>
-    </row>
-    <row r="1572">
-      <c r="A1572" s="11"/>
-      <c r="C1572" s="9"/>
-      <c r="D1572" s="2"/>
-    </row>
-    <row r="1573">
-      <c r="A1573" s="11"/>
-      <c r="C1573" s="9"/>
-      <c r="D1573" s="2"/>
-    </row>
-    <row r="1574">
-      <c r="A1574" s="11"/>
-      <c r="C1574" s="9"/>
-      <c r="D1574" s="2"/>
-    </row>
-    <row r="1575">
-      <c r="A1575" s="11"/>
-      <c r="C1575" s="9"/>
-      <c r="D1575" s="2"/>
-    </row>
-    <row r="1576">
-      <c r="A1576" s="11"/>
-      <c r="C1576" s="9"/>
-      <c r="D1576" s="2"/>
-    </row>
-    <row r="1577">
-      <c r="A1577" s="11"/>
-      <c r="C1577" s="9"/>
-      <c r="D1577" s="2"/>
-    </row>
-    <row r="1578">
-      <c r="A1578" s="11"/>
-      <c r="C1578" s="9"/>
-      <c r="D1578" s="2"/>
-    </row>
-    <row r="1579">
-      <c r="A1579" s="11"/>
-      <c r="C1579" s="9"/>
-      <c r="D1579" s="2"/>
-    </row>
-    <row r="1580">
-      <c r="A1580" s="11"/>
-      <c r="C1580" s="9"/>
-      <c r="D1580" s="2"/>
-    </row>
-    <row r="1581">
-      <c r="A1581" s="11"/>
-      <c r="C1581" s="9"/>
-      <c r="D1581" s="2"/>
-    </row>
-    <row r="1582">
-      <c r="A1582" s="11"/>
-      <c r="C1582" s="9"/>
-      <c r="D1582" s="2"/>
-    </row>
-    <row r="1583">
-      <c r="A1583" s="11"/>
-      <c r="C1583" s="9"/>
-      <c r="D1583" s="2"/>
-    </row>
-    <row r="1584">
-      <c r="A1584" s="11"/>
-      <c r="C1584" s="9"/>
-      <c r="D1584" s="2"/>
-    </row>
-    <row r="1585">
-      <c r="A1585" s="11"/>
-      <c r="C1585" s="9"/>
-      <c r="D1585" s="2"/>
-    </row>
-    <row r="1586">
-      <c r="A1586" s="11"/>
-      <c r="C1586" s="9"/>
-      <c r="D1586" s="2"/>
-    </row>
-    <row r="1587">
-      <c r="A1587" s="11"/>
-      <c r="C1587" s="9"/>
-      <c r="D1587" s="2"/>
-    </row>
-    <row r="1588">
-      <c r="A1588" s="11"/>
-      <c r="C1588" s="9"/>
-      <c r="D1588" s="2"/>
-    </row>
-    <row r="1589">
-      <c r="A1589" s="11"/>
-      <c r="C1589" s="9"/>
-      <c r="D1589" s="2"/>
-    </row>
-    <row r="1590">
-      <c r="A1590" s="11"/>
-      <c r="C1590" s="9"/>
-      <c r="D1590" s="2"/>
-    </row>
-    <row r="1591">
-      <c r="A1591" s="11"/>
-      <c r="C1591" s="9"/>
-      <c r="D1591" s="2"/>
-    </row>
-    <row r="1592">
-      <c r="A1592" s="11"/>
-      <c r="C1592" s="9"/>
-      <c r="D1592" s="2"/>
-    </row>
-    <row r="1593">
-      <c r="A1593" s="11"/>
-      <c r="C1593" s="9"/>
-      <c r="D1593" s="2"/>
-    </row>
-    <row r="1594">
-      <c r="A1594" s="11"/>
-      <c r="C1594" s="9"/>
-      <c r="D1594" s="2"/>
-    </row>
-    <row r="1595">
-      <c r="A1595" s="11"/>
-      <c r="C1595" s="9"/>
-      <c r="D1595" s="2"/>
-    </row>
-    <row r="1596">
-      <c r="A1596" s="11"/>
-      <c r="C1596" s="9"/>
-      <c r="D1596" s="2"/>
-    </row>
-    <row r="1597">
-      <c r="A1597" s="11"/>
-      <c r="C1597" s="9"/>
-      <c r="D1597" s="2"/>
-    </row>
-    <row r="1598">
-      <c r="A1598" s="11"/>
-      <c r="C1598" s="9"/>
-      <c r="D1598" s="2"/>
-    </row>
-    <row r="1599">
-      <c r="A1599" s="11"/>
-      <c r="C1599" s="9"/>
-      <c r="D1599" s="2"/>
-    </row>
-    <row r="1600">
-      <c r="A1600" s="11"/>
-      <c r="C1600" s="9"/>
-      <c r="D1600" s="2"/>
-    </row>
-    <row r="1601">
-      <c r="A1601" s="11"/>
-      <c r="C1601" s="9"/>
-      <c r="D1601" s="2"/>
-    </row>
-    <row r="1602">
-      <c r="A1602" s="11"/>
-      <c r="C1602" s="9"/>
-      <c r="D1602" s="2"/>
-    </row>
-    <row r="1603">
-      <c r="A1603" s="11"/>
-      <c r="C1603" s="9"/>
-      <c r="D1603" s="2"/>
-    </row>
-    <row r="1604">
-      <c r="A1604" s="11"/>
-      <c r="C1604" s="9"/>
-      <c r="D1604" s="2"/>
-    </row>
-    <row r="1605">
-      <c r="A1605" s="11"/>
-      <c r="C1605" s="9"/>
-      <c r="D1605" s="2"/>
-    </row>
-    <row r="1606">
-      <c r="A1606" s="11"/>
-      <c r="C1606" s="9"/>
-      <c r="D1606" s="2"/>
-    </row>
-    <row r="1607">
-      <c r="A1607" s="11"/>
-      <c r="C1607" s="9"/>
-      <c r="D1607" s="2"/>
-    </row>
-    <row r="1608">
-      <c r="A1608" s="11"/>
-      <c r="C1608" s="9"/>
-      <c r="D1608" s="2"/>
-    </row>
-    <row r="1609">
-      <c r="A1609" s="11"/>
-      <c r="C1609" s="9"/>
-      <c r="D1609" s="2"/>
-    </row>
-    <row r="1610">
-      <c r="A1610" s="11"/>
-      <c r="C1610" s="9"/>
-      <c r="D1610" s="2"/>
-    </row>
-    <row r="1611">
-      <c r="A1611" s="11"/>
-      <c r="C1611" s="9"/>
-      <c r="D1611" s="2"/>
-    </row>
-    <row r="1612">
-      <c r="A1612" s="11"/>
-      <c r="C1612" s="9"/>
-      <c r="D1612" s="2"/>
-    </row>
-    <row r="1613">
-      <c r="A1613" s="11"/>
-      <c r="C1613" s="9"/>
-      <c r="D1613" s="2"/>
-    </row>
-    <row r="1614">
-      <c r="A1614" s="11"/>
-      <c r="C1614" s="9"/>
-      <c r="D1614" s="2"/>
-    </row>
-    <row r="1615">
-      <c r="A1615" s="11"/>
-      <c r="C1615" s="9"/>
-      <c r="D1615" s="2"/>
-    </row>
-    <row r="1616">
-      <c r="A1616" s="11"/>
-      <c r="C1616" s="9"/>
-      <c r="D1616" s="2"/>
-    </row>
-    <row r="1617">
-      <c r="A1617" s="11"/>
-      <c r="C1617" s="9"/>
-      <c r="D1617" s="2"/>
-    </row>
-    <row r="1618">
-      <c r="A1618" s="11"/>
-      <c r="C1618" s="9"/>
-      <c r="D1618" s="2"/>
-    </row>
-    <row r="1619">
-      <c r="A1619" s="11"/>
-      <c r="C1619" s="9"/>
-      <c r="D1619" s="2"/>
-    </row>
-    <row r="1620">
-      <c r="A1620" s="11"/>
-      <c r="C1620" s="9"/>
-      <c r="D1620" s="2"/>
-    </row>
-    <row r="1621">
-      <c r="A1621" s="11"/>
-      <c r="C1621" s="9"/>
-      <c r="D1621" s="2"/>
-    </row>
-    <row r="1622">
-      <c r="A1622" s="11"/>
-      <c r="C1622" s="9"/>
-      <c r="D1622" s="2"/>
-    </row>
-    <row r="1623">
-      <c r="A1623" s="11"/>
-      <c r="C1623" s="9"/>
-      <c r="D1623" s="2"/>
-    </row>
-    <row r="1624">
-      <c r="A1624" s="11"/>
-      <c r="C1624" s="9"/>
-      <c r="D1624" s="2"/>
-    </row>
-    <row r="1625">
-      <c r="A1625" s="11"/>
-      <c r="C1625" s="9"/>
-      <c r="D1625" s="2"/>
-    </row>
-    <row r="1626">
-      <c r="A1626" s="11"/>
-      <c r="C1626" s="9"/>
-      <c r="D1626" s="2"/>
-    </row>
-    <row r="1627">
-      <c r="A1627" s="11"/>
-      <c r="C1627" s="9"/>
-      <c r="D1627" s="2"/>
-    </row>
-    <row r="1628">
-      <c r="A1628" s="11"/>
-      <c r="C1628" s="9"/>
-      <c r="D1628" s="2"/>
-    </row>
-    <row r="1629">
-      <c r="A1629" s="11"/>
-      <c r="C1629" s="9"/>
-      <c r="D1629" s="2"/>
-    </row>
-    <row r="1630">
-      <c r="A1630" s="11"/>
-      <c r="C1630" s="9"/>
-      <c r="D1630" s="2"/>
-    </row>
-    <row r="1631">
-      <c r="A1631" s="11"/>
-      <c r="C1631" s="9"/>
-      <c r="D1631" s="2"/>
-    </row>
-    <row r="1632">
-      <c r="A1632" s="11"/>
-      <c r="C1632" s="9"/>
-      <c r="D1632" s="2"/>
-    </row>
-    <row r="1633">
-      <c r="A1633" s="11"/>
-      <c r="C1633" s="9"/>
-      <c r="D1633" s="2"/>
-    </row>
-    <row r="1634">
-      <c r="A1634" s="11"/>
-      <c r="C1634" s="9"/>
-      <c r="D1634" s="2"/>
-    </row>
-    <row r="1635">
-      <c r="A1635" s="11"/>
-      <c r="C1635" s="9"/>
-      <c r="D1635" s="2"/>
-    </row>
-    <row r="1636">
-      <c r="A1636" s="11"/>
-      <c r="C1636" s="9"/>
-      <c r="D1636" s="2"/>
-    </row>
-    <row r="1637">
-      <c r="A1637" s="11"/>
-      <c r="C1637" s="9"/>
-      <c r="D1637" s="2"/>
-    </row>
-    <row r="1638">
-      <c r="A1638" s="11"/>
-      <c r="C1638" s="9"/>
-      <c r="D1638" s="2"/>
-    </row>
-    <row r="1639">
-      <c r="A1639" s="11"/>
-      <c r="C1639" s="9"/>
-      <c r="D1639" s="2"/>
-    </row>
-    <row r="1640">
-      <c r="A1640" s="11"/>
-      <c r="C1640" s="9"/>
-      <c r="D1640" s="2"/>
-    </row>
-    <row r="1641">
-      <c r="A1641" s="11"/>
-      <c r="C1641" s="9"/>
-      <c r="D1641" s="2"/>
-    </row>
-    <row r="1642">
-      <c r="A1642" s="11"/>
-      <c r="C1642" s="9"/>
-      <c r="D1642" s="2"/>
-    </row>
-    <row r="1643">
-      <c r="A1643" s="11"/>
-      <c r="C1643" s="9"/>
-      <c r="D1643" s="2"/>
-    </row>
-    <row r="1644">
-      <c r="A1644" s="11"/>
-      <c r="C1644" s="9"/>
-      <c r="D1644" s="2"/>
-    </row>
-    <row r="1645">
-      <c r="A1645" s="11"/>
-      <c r="C1645" s="9"/>
-      <c r="D1645" s="2"/>
-    </row>
-    <row r="1646">
-      <c r="A1646" s="11"/>
-      <c r="C1646" s="9"/>
-      <c r="D1646" s="2"/>
-    </row>
-    <row r="1647">
-      <c r="A1647" s="11"/>
-      <c r="C1647" s="9"/>
-      <c r="D1647" s="2"/>
-    </row>
-    <row r="1648">
-      <c r="A1648" s="11"/>
-      <c r="C1648" s="9"/>
-      <c r="D1648" s="2"/>
-    </row>
-    <row r="1649">
-      <c r="A1649" s="11"/>
-      <c r="C1649" s="9"/>
-      <c r="D1649" s="2"/>
-    </row>
-    <row r="1650">
-      <c r="A1650" s="11"/>
-      <c r="C1650" s="9"/>
-      <c r="D1650" s="2"/>
-    </row>
-    <row r="1651">
-      <c r="A1651" s="11"/>
-      <c r="C1651" s="9"/>
-      <c r="D1651" s="2"/>
-    </row>
-    <row r="1652">
-      <c r="A1652" s="11"/>
-      <c r="C1652" s="9"/>
-      <c r="D1652" s="2"/>
-    </row>
-    <row r="1653">
-      <c r="A1653" s="11"/>
-      <c r="C1653" s="9"/>
-      <c r="D1653" s="2"/>
-    </row>
-    <row r="1654">
-      <c r="A1654" s="11"/>
-      <c r="C1654" s="9"/>
-      <c r="D1654" s="2"/>
-    </row>
-    <row r="1655">
-      <c r="A1655" s="11"/>
-      <c r="C1655" s="9"/>
-      <c r="D1655" s="2"/>
-    </row>
-    <row r="1656">
-      <c r="A1656" s="11"/>
-      <c r="C1656" s="9"/>
-      <c r="D1656" s="2"/>
-    </row>
-    <row r="1657">
-      <c r="A1657" s="11"/>
-      <c r="C1657" s="9"/>
-      <c r="D1657" s="2"/>
-    </row>
-    <row r="1658">
-      <c r="A1658" s="11"/>
-      <c r="C1658" s="9"/>
-      <c r="D1658" s="2"/>
-    </row>
-    <row r="1659">
-      <c r="A1659" s="11"/>
-      <c r="C1659" s="9"/>
-      <c r="D1659" s="2"/>
-    </row>
-    <row r="1660">
-      <c r="A1660" s="11"/>
-      <c r="C1660" s="9"/>
-      <c r="D1660" s="2"/>
-    </row>
-    <row r="1661">
-      <c r="A1661" s="11"/>
-      <c r="C1661" s="9"/>
-      <c r="D1661" s="2"/>
-    </row>
-    <row r="1662">
-      <c r="A1662" s="11"/>
-      <c r="C1662" s="9"/>
-      <c r="D1662" s="2"/>
-    </row>
-    <row r="1663">
-      <c r="A1663" s="11"/>
-      <c r="C1663" s="9"/>
-      <c r="D1663" s="2"/>
-    </row>
-    <row r="1664">
-      <c r="A1664" s="11"/>
-      <c r="C1664" s="9"/>
-      <c r="D1664" s="2"/>
-    </row>
-    <row r="1665">
-      <c r="A1665" s="11"/>
-      <c r="C1665" s="9"/>
-      <c r="D1665" s="2"/>
-    </row>
-    <row r="1666">
-      <c r="A1666" s="11"/>
-      <c r="C1666" s="9"/>
-      <c r="D1666" s="2"/>
-    </row>
-    <row r="1667">
-      <c r="A1667" s="11"/>
-      <c r="C1667" s="9"/>
-      <c r="D1667" s="2"/>
-    </row>
-    <row r="1668">
-      <c r="A1668" s="11"/>
-      <c r="C1668" s="9"/>
-      <c r="D1668" s="2"/>
-    </row>
-    <row r="1669">
-      <c r="A1669" s="11"/>
-      <c r="C1669" s="9"/>
-      <c r="D1669" s="2"/>
-    </row>
-    <row r="1670">
-      <c r="A1670" s="11"/>
-      <c r="C1670" s="9"/>
-      <c r="D1670" s="2"/>
-    </row>
-    <row r="1671">
-      <c r="A1671" s="11"/>
-      <c r="C1671" s="9"/>
-      <c r="D1671" s="2"/>
-    </row>
-    <row r="1672">
-      <c r="A1672" s="11"/>
-      <c r="C1672" s="9"/>
-      <c r="D1672" s="2"/>
-    </row>
-    <row r="1673">
-      <c r="A1673" s="11"/>
-      <c r="C1673" s="9"/>
-      <c r="D1673" s="2"/>
-    </row>
-    <row r="1674">
-      <c r="A1674" s="11"/>
-      <c r="C1674" s="9"/>
-      <c r="D1674" s="2"/>
-    </row>
-    <row r="1675">
-      <c r="A1675" s="11"/>
-      <c r="C1675" s="9"/>
-      <c r="D1675" s="2"/>
-    </row>
-    <row r="1676">
-      <c r="A1676" s="11"/>
-      <c r="C1676" s="9"/>
-      <c r="D1676" s="2"/>
-    </row>
-    <row r="1677">
-      <c r="A1677" s="11"/>
-      <c r="C1677" s="9"/>
-      <c r="D1677" s="2"/>
-    </row>
-    <row r="1678">
-      <c r="A1678" s="11"/>
-      <c r="C1678" s="9"/>
-      <c r="D1678" s="2"/>
-    </row>
-    <row r="1679">
-      <c r="A1679" s="11"/>
-      <c r="C1679" s="9"/>
-      <c r="D1679" s="2"/>
-    </row>
-    <row r="1680">
-      <c r="A1680" s="11"/>
-      <c r="C1680" s="9"/>
-      <c r="D1680" s="2"/>
-    </row>
-    <row r="1681">
-      <c r="A1681" s="11"/>
-      <c r="C1681" s="9"/>
-      <c r="D1681" s="2"/>
-    </row>
-    <row r="1682">
-      <c r="A1682" s="11"/>
-      <c r="C1682" s="9"/>
-      <c r="D1682" s="2"/>
-    </row>
-    <row r="1683">
-      <c r="A1683" s="11"/>
-      <c r="C1683" s="9"/>
-      <c r="D1683" s="2"/>
-    </row>
-    <row r="1684">
-      <c r="A1684" s="11"/>
-      <c r="C1684" s="9"/>
-      <c r="D1684" s="2"/>
-    </row>
-    <row r="1685">
-      <c r="A1685" s="11"/>
-      <c r="C1685" s="9"/>
-      <c r="D1685" s="2"/>
-    </row>
-    <row r="1686">
-      <c r="A1686" s="11"/>
-      <c r="C1686" s="9"/>
-      <c r="D1686" s="2"/>
-    </row>
-    <row r="1687">
-      <c r="A1687" s="11"/>
-      <c r="C1687" s="9"/>
-      <c r="D1687" s="2"/>
-    </row>
-    <row r="1688">
-      <c r="A1688" s="11"/>
-      <c r="C1688" s="9"/>
-      <c r="D1688" s="2"/>
-    </row>
-    <row r="1689">
-      <c r="A1689" s="11"/>
-      <c r="C1689" s="9"/>
-      <c r="D1689" s="2"/>
-    </row>
-    <row r="1690">
-      <c r="A1690" s="11"/>
-      <c r="C1690" s="9"/>
-      <c r="D1690" s="2"/>
-    </row>
-    <row r="1691">
-      <c r="A1691" s="11"/>
-      <c r="C1691" s="9"/>
-      <c r="D1691" s="2"/>
-    </row>
-    <row r="1692">
-      <c r="A1692" s="11"/>
-      <c r="C1692" s="9"/>
-      <c r="D1692" s="2"/>
-    </row>
-    <row r="1693">
-      <c r="A1693" s="11"/>
-      <c r="C1693" s="9"/>
-      <c r="D1693" s="2"/>
-    </row>
-    <row r="1694">
-      <c r="A1694" s="11"/>
-      <c r="C1694" s="9"/>
-      <c r="D1694" s="2"/>
-    </row>
-    <row r="1695">
-      <c r="A1695" s="11"/>
-      <c r="C1695" s="9"/>
-      <c r="D1695" s="2"/>
-    </row>
-    <row r="1696">
-      <c r="A1696" s="11"/>
-      <c r="C1696" s="9"/>
-      <c r="D1696" s="2"/>
-    </row>
-    <row r="1697">
-      <c r="A1697" s="11"/>
-      <c r="C1697" s="9"/>
-      <c r="D1697" s="2"/>
-    </row>
-    <row r="1698">
-      <c r="A1698" s="11"/>
-      <c r="C1698" s="9"/>
-      <c r="D1698" s="2"/>
-    </row>
-    <row r="1699">
-      <c r="A1699" s="11"/>
-      <c r="C1699" s="9"/>
-      <c r="D1699" s="2"/>
-    </row>
-    <row r="1700">
-      <c r="A1700" s="11"/>
-      <c r="C1700" s="9"/>
-      <c r="D1700" s="2"/>
-    </row>
-    <row r="1701">
-      <c r="A1701" s="11"/>
-      <c r="C1701" s="9"/>
-      <c r="D1701" s="2"/>
-    </row>
-    <row r="1702">
-      <c r="A1702" s="11"/>
-      <c r="C1702" s="9"/>
-      <c r="D1702" s="2"/>
-    </row>
-    <row r="1703">
-      <c r="A1703" s="11"/>
-      <c r="C1703" s="9"/>
-      <c r="D1703" s="2"/>
-    </row>
-    <row r="1704">
-      <c r="A1704" s="11"/>
-      <c r="C1704" s="9"/>
-      <c r="D1704" s="2"/>
-    </row>
-    <row r="1705">
-      <c r="A1705" s="11"/>
-      <c r="C1705" s="9"/>
-      <c r="D1705" s="2"/>
-    </row>
-    <row r="1706">
-      <c r="A1706" s="11"/>
-      <c r="C1706" s="9"/>
-      <c r="D1706" s="2"/>
-    </row>
-    <row r="1707">
-      <c r="A1707" s="11"/>
-      <c r="C1707" s="9"/>
-      <c r="D1707" s="2"/>
-    </row>
-    <row r="1708">
-      <c r="A1708" s="11"/>
-      <c r="C1708" s="9"/>
-      <c r="D1708" s="2"/>
-    </row>
-    <row r="1709">
-      <c r="A1709" s="11"/>
-      <c r="C1709" s="9"/>
-      <c r="D1709" s="2"/>
-    </row>
-    <row r="1710">
-      <c r="A1710" s="11"/>
-      <c r="C1710" s="9"/>
-      <c r="D1710" s="2"/>
-    </row>
-    <row r="1711">
-      <c r="A1711" s="11"/>
-      <c r="C1711" s="9"/>
-      <c r="D1711" s="2"/>
-    </row>
-    <row r="1712">
-      <c r="A1712" s="11"/>
-      <c r="C1712" s="9"/>
-      <c r="D1712" s="2"/>
-    </row>
-    <row r="1713">
-      <c r="A1713" s="11"/>
-      <c r="C1713" s="9"/>
-      <c r="D1713" s="2"/>
-    </row>
-    <row r="1714">
-      <c r="A1714" s="11"/>
-      <c r="C1714" s="9"/>
-      <c r="D1714" s="2"/>
-    </row>
-    <row r="1715">
-      <c r="A1715" s="11"/>
-      <c r="C1715" s="9"/>
-      <c r="D1715" s="2"/>
-    </row>
-    <row r="1716">
-      <c r="A1716" s="11"/>
-      <c r="C1716" s="9"/>
-      <c r="D1716" s="2"/>
-    </row>
-    <row r="1717">
-      <c r="A1717" s="11"/>
-      <c r="C1717" s="9"/>
-      <c r="D1717" s="2"/>
-    </row>
-    <row r="1718">
-      <c r="A1718" s="11"/>
-      <c r="C1718" s="9"/>
-      <c r="D1718" s="2"/>
-    </row>
-    <row r="1719">
-      <c r="A1719" s="11"/>
-      <c r="C1719" s="9"/>
-      <c r="D1719" s="2"/>
-    </row>
-    <row r="1720">
-      <c r="A1720" s="11"/>
-      <c r="C1720" s="9"/>
-      <c r="D1720" s="2"/>
-    </row>
-    <row r="1721">
-      <c r="A1721" s="11"/>
-      <c r="C1721" s="9"/>
-      <c r="D1721" s="2"/>
-    </row>
-    <row r="1722">
-      <c r="A1722" s="11"/>
-      <c r="C1722" s="9"/>
-      <c r="D1722" s="2"/>
-    </row>
-    <row r="1723">
-      <c r="A1723" s="11"/>
-      <c r="C1723" s="9"/>
-      <c r="D1723" s="2"/>
-    </row>
-    <row r="1724">
-      <c r="A1724" s="11"/>
-      <c r="C1724" s="9"/>
-      <c r="D1724" s="2"/>
-    </row>
-    <row r="1725">
-      <c r="A1725" s="11"/>
-      <c r="C1725" s="9"/>
-      <c r="D1725" s="2"/>
-    </row>
-    <row r="1726">
-      <c r="A1726" s="11"/>
-      <c r="C1726" s="9"/>
-      <c r="D1726" s="2"/>
-    </row>
-    <row r="1727">
-      <c r="A1727" s="11"/>
-      <c r="C1727" s="9"/>
-      <c r="D1727" s="2"/>
-    </row>
-    <row r="1728">
-      <c r="A1728" s="11"/>
-      <c r="C1728" s="9"/>
-      <c r="D1728" s="2"/>
-    </row>
-    <row r="1729">
-      <c r="A1729" s="11"/>
-      <c r="C1729" s="9"/>
-      <c r="D1729" s="2"/>
-    </row>
-    <row r="1730">
-      <c r="A1730" s="11"/>
-      <c r="C1730" s="9"/>
-      <c r="D1730" s="2"/>
-    </row>
-    <row r="1731">
-      <c r="A1731" s="11"/>
-      <c r="C1731" s="9"/>
-      <c r="D1731" s="2"/>
-    </row>
-    <row r="1732">
-      <c r="A1732" s="11"/>
-      <c r="C1732" s="9"/>
-      <c r="D1732" s="2"/>
-    </row>
-    <row r="1733">
-      <c r="A1733" s="11"/>
-      <c r="C1733" s="9"/>
-      <c r="D1733" s="2"/>
-    </row>
-    <row r="1734">
-      <c r="A1734" s="11"/>
-      <c r="C1734" s="9"/>
-      <c r="D1734" s="2"/>
-    </row>
-    <row r="1735">
-      <c r="A1735" s="11"/>
-      <c r="C1735" s="9"/>
-      <c r="D1735" s="2"/>
-    </row>
-    <row r="1736">
-      <c r="A1736" s="11"/>
-      <c r="C1736" s="9"/>
-      <c r="D1736" s="2"/>
-    </row>
-    <row r="1737">
-      <c r="A1737" s="11"/>
-      <c r="C1737" s="9"/>
-      <c r="D1737" s="2"/>
-    </row>
-    <row r="1738">
-      <c r="A1738" s="11"/>
-      <c r="C1738" s="9"/>
-      <c r="D1738" s="2"/>
-    </row>
-    <row r="1739">
-      <c r="A1739" s="11"/>
-      <c r="C1739" s="9"/>
-      <c r="D1739" s="2"/>
-    </row>
-    <row r="1740">
-      <c r="A1740" s="11"/>
-      <c r="C1740" s="9"/>
-      <c r="D1740" s="2"/>
-    </row>
-    <row r="1741">
-      <c r="A1741" s="11"/>
-      <c r="C1741" s="9"/>
-      <c r="D1741" s="2"/>
-    </row>
-    <row r="1742">
-      <c r="A1742" s="11"/>
-      <c r="C1742" s="9"/>
-      <c r="D1742" s="2"/>
-    </row>
-    <row r="1743">
-      <c r="A1743" s="11"/>
-      <c r="C1743" s="9"/>
-      <c r="D1743" s="2"/>
-    </row>
-    <row r="1744">
-      <c r="A1744" s="11"/>
-      <c r="C1744" s="9"/>
-      <c r="D1744" s="2"/>
-    </row>
-    <row r="1745">
-      <c r="A1745" s="11"/>
-      <c r="C1745" s="9"/>
-      <c r="D1745" s="2"/>
-    </row>
-    <row r="1746">
-      <c r="A1746" s="11"/>
-      <c r="C1746" s="9"/>
-      <c r="D1746" s="2"/>
-    </row>
-    <row r="1747">
-      <c r="A1747" s="11"/>
-      <c r="C1747" s="9"/>
-      <c r="D1747" s="2"/>
-    </row>
-    <row r="1748">
-      <c r="A1748" s="11"/>
-      <c r="C1748" s="9"/>
-      <c r="D1748" s="2"/>
-    </row>
-    <row r="1749">
-      <c r="A1749" s="11"/>
-      <c r="C1749" s="9"/>
-      <c r="D1749" s="2"/>
-    </row>
-    <row r="1750">
-      <c r="A1750" s="11"/>
-      <c r="C1750" s="9"/>
-      <c r="D1750" s="2"/>
-    </row>
-    <row r="1751">
-      <c r="A1751" s="11"/>
-      <c r="C1751" s="9"/>
-      <c r="D1751" s="2"/>
-    </row>
-    <row r="1752">
-      <c r="A1752" s="11"/>
-      <c r="C1752" s="9"/>
-      <c r="D1752" s="2"/>
-    </row>
-    <row r="1753">
-      <c r="A1753" s="11"/>
-      <c r="C1753" s="9"/>
-      <c r="D1753" s="2"/>
-    </row>
-    <row r="1754">
-      <c r="A1754" s="11"/>
-      <c r="C1754" s="9"/>
-      <c r="D1754" s="2"/>
-    </row>
-    <row r="1755">
-      <c r="A1755" s="11"/>
-      <c r="C1755" s="9"/>
-      <c r="D1755" s="2"/>
-    </row>
-    <row r="1756">
-      <c r="A1756" s="11"/>
-      <c r="C1756" s="9"/>
-      <c r="D1756" s="2"/>
-    </row>
-    <row r="1757">
-      <c r="A1757" s="11"/>
-      <c r="C1757" s="9"/>
-      <c r="D1757" s="2"/>
-    </row>
-    <row r="1758">
-      <c r="A1758" s="11"/>
-      <c r="C1758" s="9"/>
-      <c r="D1758" s="2"/>
-    </row>
-    <row r="1759">
-      <c r="A1759" s="11"/>
-      <c r="C1759" s="9"/>
-      <c r="D1759" s="2"/>
-    </row>
-    <row r="1760">
-      <c r="A1760" s="11"/>
-      <c r="C1760" s="9"/>
-      <c r="D1760" s="2"/>
-    </row>
-    <row r="1761">
-      <c r="A1761" s="11"/>
-      <c r="C1761" s="9"/>
-      <c r="D1761" s="2"/>
-    </row>
-    <row r="1762">
-      <c r="A1762" s="11"/>
-      <c r="C1762" s="9"/>
-      <c r="D1762" s="2"/>
-    </row>
-    <row r="1763">
-      <c r="A1763" s="11"/>
-      <c r="C1763" s="9"/>
-      <c r="D1763" s="2"/>
-    </row>
-    <row r="1764">
-      <c r="A1764" s="11"/>
-      <c r="C1764" s="9"/>
-      <c r="D1764" s="2"/>
-    </row>
-    <row r="1765">
-      <c r="A1765" s="11"/>
-      <c r="C1765" s="9"/>
-      <c r="D1765" s="2"/>
-    </row>
-    <row r="1766">
-      <c r="A1766" s="11"/>
-      <c r="C1766" s="9"/>
-      <c r="D1766" s="2"/>
-    </row>
-    <row r="1767">
-      <c r="A1767" s="11"/>
-      <c r="C1767" s="9"/>
-      <c r="D1767" s="2"/>
-    </row>
-    <row r="1768">
-      <c r="A1768" s="11"/>
-      <c r="C1768" s="9"/>
-      <c r="D1768" s="2"/>
-    </row>
-    <row r="1769">
-      <c r="A1769" s="11"/>
-      <c r="C1769" s="9"/>
-      <c r="D1769" s="2"/>
-    </row>
-    <row r="1770">
-      <c r="A1770" s="11"/>
-      <c r="C1770" s="9"/>
-      <c r="D1770" s="2"/>
-    </row>
-    <row r="1771">
-      <c r="A1771" s="11"/>
-      <c r="C1771" s="9"/>
-      <c r="D1771" s="2"/>
-    </row>
-    <row r="1772">
-      <c r="A1772" s="11"/>
-      <c r="C1772" s="9"/>
-      <c r="D1772" s="2"/>
-    </row>
-    <row r="1773">
-      <c r="A1773" s="11"/>
-      <c r="C1773" s="9"/>
-      <c r="D1773" s="2"/>
-    </row>
-    <row r="1774">
-      <c r="A1774" s="11"/>
-      <c r="C1774" s="9"/>
-      <c r="D1774" s="2"/>
-    </row>
-    <row r="1775">
-      <c r="A1775" s="11"/>
-      <c r="C1775" s="9"/>
-      <c r="D1775" s="2"/>
-    </row>
-    <row r="1776">
-      <c r="A1776" s="11"/>
-      <c r="C1776" s="9"/>
-      <c r="D1776" s="2"/>
-    </row>
-    <row r="1777">
-      <c r="A1777" s="11"/>
-      <c r="C1777" s="9"/>
-      <c r="D1777" s="2"/>
-    </row>
-    <row r="1778">
-      <c r="A1778" s="11"/>
-      <c r="C1778" s="9"/>
-      <c r="D1778" s="2"/>
-    </row>
-    <row r="1779">
-      <c r="A1779" s="11"/>
-      <c r="C1779" s="9"/>
-      <c r="D1779" s="2"/>
-    </row>
-    <row r="1780">
-      <c r="A1780" s="11"/>
-      <c r="C1780" s="9"/>
-      <c r="D1780" s="2"/>
-    </row>
-    <row r="1781">
-      <c r="A1781" s="11"/>
-      <c r="C1781" s="9"/>
-      <c r="D1781" s="2"/>
-    </row>
-    <row r="1782">
-      <c r="A1782" s="11"/>
-      <c r="C1782" s="9"/>
-      <c r="D1782" s="2"/>
-    </row>
-    <row r="1783">
-      <c r="A1783" s="11"/>
-      <c r="C1783" s="9"/>
-      <c r="D1783" s="2"/>
-    </row>
-    <row r="1784">
-      <c r="A1784" s="11"/>
-      <c r="C1784" s="9"/>
-      <c r="D1784" s="2"/>
-    </row>
-    <row r="1785">
-      <c r="A1785" s="11"/>
-      <c r="C1785" s="9"/>
-      <c r="D1785" s="2"/>
-    </row>
-    <row r="1786">
-      <c r="A1786" s="11"/>
-      <c r="C1786" s="9"/>
-      <c r="D1786" s="2"/>
-    </row>
-    <row r="1787">
-      <c r="A1787" s="11"/>
-      <c r="C1787" s="9"/>
-      <c r="D1787" s="2"/>
-    </row>
-    <row r="1788">
-      <c r="A1788" s="11"/>
-      <c r="C1788" s="9"/>
-      <c r="D1788" s="2"/>
-    </row>
-    <row r="1789">
-      <c r="A1789" s="11"/>
-      <c r="C1789" s="9"/>
-      <c r="D1789" s="2"/>
-    </row>
-    <row r="1790">
-      <c r="A1790" s="11"/>
-      <c r="C1790" s="9"/>
-      <c r="D1790" s="2"/>
-    </row>
-    <row r="1791">
-      <c r="A1791" s="11"/>
-      <c r="C1791" s="9"/>
-      <c r="D1791" s="2"/>
-    </row>
-    <row r="1792">
-      <c r="A1792" s="11"/>
-      <c r="C1792" s="9"/>
-      <c r="D1792" s="2"/>
-    </row>
-    <row r="1793">
-      <c r="A1793" s="11"/>
-      <c r="C1793" s="9"/>
-      <c r="D1793" s="2"/>
-    </row>
-    <row r="1794">
-      <c r="A1794" s="11"/>
-      <c r="C1794" s="9"/>
-      <c r="D1794" s="2"/>
-    </row>
-    <row r="1795">
-      <c r="A1795" s="11"/>
-      <c r="C1795" s="9"/>
-      <c r="D1795" s="2"/>
-    </row>
-    <row r="1796">
-      <c r="A1796" s="11"/>
-      <c r="C1796" s="9"/>
-      <c r="D1796" s="2"/>
-    </row>
-    <row r="1797">
-      <c r="A1797" s="11"/>
-      <c r="C1797" s="9"/>
-      <c r="D1797" s="2"/>
-    </row>
-    <row r="1798">
-      <c r="A1798" s="11"/>
-      <c r="C1798" s="9"/>
-      <c r="D1798" s="2"/>
-    </row>
-    <row r="1799">
-      <c r="A1799" s="11"/>
-      <c r="C1799" s="9"/>
-      <c r="D1799" s="2"/>
-    </row>
-    <row r="1800">
-      <c r="A1800" s="11"/>
-      <c r="C1800" s="9"/>
-      <c r="D1800" s="2"/>
-    </row>
-    <row r="1801">
-      <c r="A1801" s="11"/>
-      <c r="C1801" s="9"/>
-      <c r="D1801" s="2"/>
-    </row>
-    <row r="1802">
-      <c r="A1802" s="11"/>
-      <c r="C1802" s="9"/>
-      <c r="D1802" s="2"/>
-    </row>
-    <row r="1803">
-      <c r="A1803" s="11"/>
-      <c r="C1803" s="9"/>
-      <c r="D1803" s="2"/>
-    </row>
-    <row r="1804">
-      <c r="A1804" s="11"/>
-      <c r="C1804" s="9"/>
-      <c r="D1804" s="2"/>
-    </row>
-    <row r="1805">
-      <c r="A1805" s="11"/>
-      <c r="C1805" s="9"/>
-      <c r="D1805" s="2"/>
-    </row>
-    <row r="1806">
-      <c r="A1806" s="11"/>
-      <c r="C1806" s="9"/>
-      <c r="D1806" s="2"/>
-    </row>
-    <row r="1807">
-      <c r="A1807" s="11"/>
-      <c r="C1807" s="9"/>
-      <c r="D1807" s="2"/>
-    </row>
-    <row r="1808">
-      <c r="A1808" s="11"/>
-      <c r="C1808" s="9"/>
-      <c r="D1808" s="2"/>
-    </row>
-    <row r="1809">
-      <c r="A1809" s="11"/>
-      <c r="C1809" s="9"/>
-      <c r="D1809" s="2"/>
-    </row>
-    <row r="1810">
-      <c r="A1810" s="11"/>
-      <c r="C1810" s="9"/>
-      <c r="D1810" s="2"/>
-    </row>
-    <row r="1811">
-      <c r="A1811" s="11"/>
-      <c r="C1811" s="9"/>
-      <c r="D1811" s="2"/>
-    </row>
-    <row r="1812">
-      <c r="A1812" s="11"/>
-      <c r="C1812" s="9"/>
-      <c r="D1812" s="2"/>
-    </row>
-    <row r="1813">
-      <c r="A1813" s="11"/>
-      <c r="C1813" s="9"/>
-      <c r="D1813" s="2"/>
-    </row>
-    <row r="1814">
-      <c r="A1814" s="11"/>
-      <c r="C1814" s="9"/>
-      <c r="D1814" s="2"/>
-    </row>
-    <row r="1815">
-      <c r="A1815" s="11"/>
-      <c r="C1815" s="9"/>
-      <c r="D1815" s="2"/>
-    </row>
-    <row r="1816">
-      <c r="A1816" s="11"/>
-      <c r="C1816" s="9"/>
-      <c r="D1816" s="2"/>
-    </row>
-    <row r="1817">
-      <c r="A1817" s="11"/>
-      <c r="C1817" s="9"/>
-      <c r="D1817" s="2"/>
-    </row>
-    <row r="1818">
-      <c r="A1818" s="11"/>
-      <c r="C1818" s="9"/>
-      <c r="D1818" s="2"/>
-    </row>
-    <row r="1819">
-      <c r="A1819" s="11"/>
-      <c r="C1819" s="9"/>
-      <c r="D1819" s="2"/>
-    </row>
-    <row r="1820">
-      <c r="A1820" s="11"/>
-      <c r="C1820" s="9"/>
-      <c r="D1820" s="2"/>
-    </row>
-    <row r="1821">
-      <c r="A1821" s="11"/>
-      <c r="C1821" s="9"/>
-      <c r="D1821" s="2"/>
-    </row>
-    <row r="1822">
-      <c r="A1822" s="11"/>
-      <c r="C1822" s="9"/>
-      <c r="D1822" s="2"/>
-    </row>
-    <row r="1823">
-      <c r="A1823" s="11"/>
-      <c r="C1823" s="9"/>
-      <c r="D1823" s="2"/>
-    </row>
-    <row r="1824">
-      <c r="A1824" s="11"/>
-      <c r="C1824" s="9"/>
-      <c r="D1824" s="2"/>
-    </row>
-    <row r="1825">
-      <c r="A1825" s="11"/>
-      <c r="C1825" s="9"/>
-      <c r="D1825" s="2"/>
-    </row>
-    <row r="1826">
-      <c r="A1826" s="11"/>
-      <c r="C1826" s="9"/>
-      <c r="D1826" s="2"/>
-    </row>
-    <row r="1827">
-      <c r="A1827" s="11"/>
-      <c r="C1827" s="9"/>
-      <c r="D1827" s="2"/>
-    </row>
-    <row r="1828">
-      <c r="A1828" s="11"/>
-      <c r="C1828" s="9"/>
-      <c r="D1828" s="2"/>
-    </row>
-    <row r="1829">
-      <c r="A1829" s="11"/>
-      <c r="C1829" s="9"/>
-      <c r="D1829" s="2"/>
-    </row>
-    <row r="1830">
-      <c r="A1830" s="11"/>
-      <c r="C1830" s="9"/>
-      <c r="D1830" s="2"/>
-    </row>
-    <row r="1831">
-      <c r="A1831" s="11"/>
-      <c r="C1831" s="9"/>
-      <c r="D1831" s="2"/>
-    </row>
-    <row r="1832">
-      <c r="A1832" s="11"/>
-      <c r="C1832" s="9"/>
-      <c r="D1832" s="2"/>
-    </row>
-    <row r="1833">
-      <c r="A1833" s="11"/>
-      <c r="C1833" s="9"/>
-      <c r="D1833" s="2"/>
-    </row>
-    <row r="1834">
-      <c r="A1834" s="11"/>
-      <c r="C1834" s="9"/>
-      <c r="D1834" s="2"/>
-    </row>
-    <row r="1835">
-      <c r="A1835" s="11"/>
-      <c r="C1835" s="9"/>
-      <c r="D1835" s="2"/>
-    </row>
-    <row r="1836">
-      <c r="A1836" s="11"/>
-      <c r="C1836" s="9"/>
-      <c r="D1836" s="2"/>
-    </row>
-    <row r="1837">
-      <c r="A1837" s="11"/>
-      <c r="C1837" s="9"/>
-      <c r="D1837" s="2"/>
-    </row>
-    <row r="1838">
-      <c r="A1838" s="11"/>
-      <c r="C1838" s="9"/>
-      <c r="D1838" s="2"/>
-    </row>
-    <row r="1839">
-      <c r="A1839" s="11"/>
-      <c r="C1839" s="9"/>
-      <c r="D1839" s="2"/>
-    </row>
-    <row r="1840">
-      <c r="A1840" s="11"/>
-      <c r="C1840" s="9"/>
-      <c r="D1840" s="2"/>
-    </row>
-    <row r="1841">
-      <c r="A1841" s="11"/>
-      <c r="C1841" s="9"/>
-      <c r="D1841" s="2"/>
-    </row>
-    <row r="1842">
-      <c r="A1842" s="11"/>
-      <c r="C1842" s="9"/>
-      <c r="D1842" s="2"/>
-    </row>
-    <row r="1843">
-      <c r="A1843" s="11"/>
-      <c r="C1843" s="9"/>
-      <c r="D1843" s="2"/>
-    </row>
-    <row r="1844">
-      <c r="A1844" s="11"/>
-      <c r="C1844" s="9"/>
-      <c r="D1844" s="2"/>
-    </row>
-    <row r="1845">
-      <c r="A1845" s="11"/>
-      <c r="C1845" s="9"/>
-      <c r="D1845" s="2"/>
-    </row>
-    <row r="1846">
-      <c r="A1846" s="11"/>
-      <c r="C1846" s="9"/>
-      <c r="D1846" s="2"/>
-    </row>
-    <row r="1847">
-      <c r="A1847" s="11"/>
-      <c r="C1847" s="9"/>
-      <c r="D1847" s="2"/>
-    </row>
-    <row r="1848">
-      <c r="A1848" s="11"/>
-      <c r="C1848" s="9"/>
-      <c r="D1848" s="2"/>
-    </row>
-    <row r="1849">
-      <c r="A1849" s="11"/>
-      <c r="C1849" s="9"/>
-      <c r="D1849" s="2"/>
-    </row>
-    <row r="1850">
-      <c r="A1850" s="11"/>
-      <c r="C1850" s="9"/>
-      <c r="D1850" s="2"/>
-    </row>
-    <row r="1851">
-      <c r="A1851" s="11"/>
-      <c r="C1851" s="9"/>
-      <c r="D1851" s="2"/>
-    </row>
-    <row r="1852">
-      <c r="A1852" s="11"/>
-      <c r="C1852" s="9"/>
-      <c r="D1852" s="2"/>
-    </row>
-    <row r="1853">
-      <c r="A1853" s="11"/>
-      <c r="C1853" s="9"/>
-      <c r="D1853" s="2"/>
-    </row>
-    <row r="1854">
-      <c r="A1854" s="11"/>
-      <c r="C1854" s="9"/>
-      <c r="D1854" s="2"/>
-    </row>
-    <row r="1855">
-      <c r="A1855" s="11"/>
-      <c r="C1855" s="9"/>
-      <c r="D1855" s="2"/>
-    </row>
-    <row r="1856">
-      <c r="A1856" s="11"/>
-      <c r="C1856" s="9"/>
-      <c r="D1856" s="2"/>
-    </row>
-    <row r="1857">
-      <c r="A1857" s="11"/>
-      <c r="C1857" s="9"/>
-      <c r="D1857" s="2"/>
-    </row>
-    <row r="1858">
-      <c r="A1858" s="11"/>
-      <c r="C1858" s="9"/>
-      <c r="D1858" s="2"/>
-    </row>
-    <row r="1859">
-      <c r="A1859" s="11"/>
-      <c r="C1859" s="9"/>
-      <c r="D1859" s="2"/>
-    </row>
-    <row r="1860">
-      <c r="A1860" s="11"/>
-      <c r="C1860" s="9"/>
-      <c r="D1860" s="2"/>
-    </row>
-    <row r="1861">
-      <c r="A1861" s="11"/>
-      <c r="C1861" s="9"/>
-      <c r="D1861" s="2"/>
-    </row>
-    <row r="1862">
-      <c r="A1862" s="11"/>
-      <c r="C1862" s="9"/>
-      <c r="D1862" s="2"/>
-    </row>
-    <row r="1863">
-      <c r="A1863" s="11"/>
-      <c r="C1863" s="9"/>
-      <c r="D1863" s="2"/>
-    </row>
-    <row r="1864">
-      <c r="A1864" s="11"/>
-      <c r="C1864" s="9"/>
-      <c r="D1864" s="2"/>
-    </row>
-    <row r="1865">
-      <c r="A1865" s="11"/>
-      <c r="C1865" s="9"/>
-      <c r="D1865" s="2"/>
-    </row>
-    <row r="1866">
-      <c r="A1866" s="11"/>
-      <c r="C1866" s="9"/>
-      <c r="D1866" s="2"/>
-    </row>
-    <row r="1867">
-      <c r="A1867" s="11"/>
-      <c r="C1867" s="9"/>
-      <c r="D1867" s="2"/>
-    </row>
-    <row r="1868">
-      <c r="A1868" s="11"/>
-      <c r="C1868" s="9"/>
-      <c r="D1868" s="2"/>
-    </row>
-    <row r="1869">
-      <c r="A1869" s="11"/>
-      <c r="C1869" s="9"/>
-      <c r="D1869" s="2"/>
-    </row>
-    <row r="1870">
-      <c r="A1870" s="11"/>
-      <c r="C1870" s="9"/>
-      <c r="D1870" s="2"/>
-    </row>
-    <row r="1871">
-      <c r="A1871" s="11"/>
-      <c r="C1871" s="9"/>
-      <c r="D1871" s="2"/>
-    </row>
-    <row r="1872">
-      <c r="A1872" s="11"/>
-      <c r="C1872" s="9"/>
-      <c r="D1872" s="2"/>
-    </row>
-    <row r="1873">
-      <c r="A1873" s="11"/>
-      <c r="C1873" s="9"/>
-      <c r="D1873" s="2"/>
-    </row>
-    <row r="1874">
-      <c r="A1874" s="11"/>
-      <c r="C1874" s="9"/>
-      <c r="D1874" s="2"/>
-    </row>
-    <row r="1875">
-      <c r="A1875" s="11"/>
-      <c r="C1875" s="9"/>
-      <c r="D1875" s="2"/>
-    </row>
-    <row r="1876">
-      <c r="A1876" s="11"/>
-      <c r="C1876" s="9"/>
-      <c r="D1876" s="2"/>
-    </row>
-    <row r="1877">
-      <c r="A1877" s="11"/>
-      <c r="C1877" s="9"/>
-      <c r="D1877" s="2"/>
-    </row>
-    <row r="1878">
-      <c r="A1878" s="11"/>
-      <c r="C1878" s="9"/>
-      <c r="D1878" s="2"/>
-    </row>
-    <row r="1879">
-      <c r="A1879" s="11"/>
-      <c r="C1879" s="9"/>
-      <c r="D1879" s="2"/>
-    </row>
-    <row r="1880">
-      <c r="A1880" s="11"/>
-      <c r="C1880" s="9"/>
-      <c r="D1880" s="2"/>
-    </row>
-    <row r="1881">
-      <c r="A1881" s="11"/>
-      <c r="C1881" s="9"/>
-      <c r="D1881" s="2"/>
-    </row>
-    <row r="1882">
-      <c r="A1882" s="11"/>
-      <c r="C1882" s="9"/>
-      <c r="D1882" s="2"/>
-    </row>
-    <row r="1883">
-      <c r="A1883" s="11"/>
-      <c r="C1883" s="9"/>
-      <c r="D1883" s="2"/>
-    </row>
-    <row r="1884">
-      <c r="A1884" s="11"/>
-      <c r="C1884" s="9"/>
-      <c r="D1884" s="2"/>
-    </row>
-    <row r="1885">
-      <c r="A1885" s="11"/>
-      <c r="C1885" s="9"/>
-      <c r="D1885" s="2"/>
-    </row>
-    <row r="1886">
-      <c r="A1886" s="11"/>
-      <c r="C1886" s="9"/>
-      <c r="D1886" s="2"/>
-    </row>
-    <row r="1887">
-      <c r="A1887" s="11"/>
-      <c r="C1887" s="9"/>
-      <c r="D1887" s="2"/>
-    </row>
-    <row r="1888">
-      <c r="A1888" s="11"/>
-      <c r="C1888" s="9"/>
-      <c r="D1888" s="2"/>
-    </row>
-    <row r="1889">
-      <c r="A1889" s="11"/>
-      <c r="C1889" s="9"/>
-      <c r="D1889" s="2"/>
-    </row>
-    <row r="1890">
-      <c r="A1890" s="11"/>
-      <c r="C1890" s="9"/>
-      <c r="D1890" s="2"/>
-    </row>
-    <row r="1891">
-      <c r="A1891" s="11"/>
-      <c r="C1891" s="9"/>
-      <c r="D1891" s="2"/>
-    </row>
-    <row r="1892">
-      <c r="A1892" s="11"/>
-      <c r="C1892" s="9"/>
-      <c r="D1892" s="2"/>
-    </row>
-    <row r="1893">
-      <c r="A1893" s="11"/>
-      <c r="C1893" s="9"/>
-      <c r="D1893" s="2"/>
-    </row>
-    <row r="1894">
-      <c r="A1894" s="11"/>
-      <c r="C1894" s="9"/>
-      <c r="D1894" s="2"/>
-    </row>
-    <row r="1895">
-      <c r="A1895" s="11"/>
-      <c r="C1895" s="9"/>
-      <c r="D1895" s="2"/>
-    </row>
-    <row r="1896">
-      <c r="A1896" s="11"/>
-      <c r="C1896" s="9"/>
-      <c r="D1896" s="2"/>
-    </row>
-    <row r="1897">
-      <c r="A1897" s="11"/>
-      <c r="C1897" s="9"/>
-      <c r="D1897" s="2"/>
-    </row>
-    <row r="1898">
-      <c r="A1898" s="11"/>
-      <c r="C1898" s="9"/>
-      <c r="D1898" s="2"/>
-    </row>
-    <row r="1899">
-      <c r="A1899" s="11"/>
-      <c r="C1899" s="9"/>
-      <c r="D1899" s="2"/>
-    </row>
-    <row r="1900">
-      <c r="A1900" s="11"/>
-      <c r="C1900" s="9"/>
-      <c r="D1900" s="2"/>
-    </row>
-    <row r="1901">
-      <c r="A1901" s="11"/>
-      <c r="C1901" s="9"/>
-      <c r="D1901" s="2"/>
-    </row>
-    <row r="1902">
-      <c r="A1902" s="11"/>
-      <c r="C1902" s="9"/>
-      <c r="D1902" s="2"/>
-    </row>
-    <row r="1903">
-      <c r="A1903" s="11"/>
-      <c r="C1903" s="9"/>
-      <c r="D1903" s="2"/>
-    </row>
-    <row r="1904">
-      <c r="A1904" s="11"/>
-      <c r="C1904" s="9"/>
-      <c r="D1904" s="2"/>
-    </row>
-    <row r="1905">
-      <c r="A1905" s="11"/>
-      <c r="C1905" s="9"/>
-      <c r="D1905" s="2"/>
-    </row>
-    <row r="1906">
-      <c r="A1906" s="11"/>
-      <c r="C1906" s="9"/>
-      <c r="D1906" s="2"/>
-    </row>
-    <row r="1907">
-      <c r="A1907" s="11"/>
-      <c r="C1907" s="9"/>
-      <c r="D1907" s="2"/>
-    </row>
-    <row r="1908">
-      <c r="A1908" s="11"/>
-      <c r="C1908" s="9"/>
-      <c r="D1908" s="2"/>
-    </row>
-    <row r="1909">
-      <c r="A1909" s="11"/>
-      <c r="C1909" s="9"/>
-      <c r="D1909" s="2"/>
-    </row>
-    <row r="1910">
-      <c r="A1910" s="11"/>
-      <c r="C1910" s="9"/>
-      <c r="D1910" s="2"/>
-    </row>
-    <row r="1911">
-      <c r="A1911" s="11"/>
-      <c r="C1911" s="9"/>
-      <c r="D1911" s="2"/>
-    </row>
-    <row r="1912">
-      <c r="A1912" s="11"/>
-      <c r="C1912" s="9"/>
-      <c r="D1912" s="2"/>
-    </row>
-    <row r="1913">
-      <c r="A1913" s="11"/>
-      <c r="C1913" s="9"/>
-      <c r="D1913" s="2"/>
-    </row>
-    <row r="1914">
-      <c r="A1914" s="11"/>
-      <c r="C1914" s="9"/>
-      <c r="D1914" s="2"/>
-    </row>
-    <row r="1915">
-      <c r="A1915" s="11"/>
-      <c r="C1915" s="9"/>
-      <c r="D1915" s="2"/>
-    </row>
-    <row r="1916">
-      <c r="A1916" s="11"/>
-      <c r="C1916" s="9"/>
-      <c r="D1916" s="2"/>
-    </row>
-    <row r="1917">
-      <c r="A1917" s="11"/>
-      <c r="C1917" s="9"/>
-      <c r="D1917" s="2"/>
-    </row>
-    <row r="1918">
-      <c r="A1918" s="11"/>
-      <c r="C1918" s="9"/>
-      <c r="D1918" s="2"/>
-    </row>
-    <row r="1919">
-      <c r="A1919" s="11"/>
-      <c r="C1919" s="9"/>
-      <c r="D1919" s="2"/>
-    </row>
-    <row r="1920">
-      <c r="A1920" s="11"/>
-      <c r="C1920" s="9"/>
-      <c r="D1920" s="2"/>
-    </row>
-    <row r="1921">
-      <c r="A1921" s="11"/>
-      <c r="C1921" s="9"/>
-      <c r="D1921" s="2"/>
-    </row>
-    <row r="1922">
-      <c r="A1922" s="11"/>
-      <c r="C1922" s="9"/>
-      <c r="D1922" s="2"/>
-    </row>
-    <row r="1923">
-      <c r="A1923" s="11"/>
-      <c r="C1923" s="9"/>
-      <c r="D1923" s="2"/>
-    </row>
-    <row r="1924">
-      <c r="A1924" s="11"/>
-      <c r="C1924" s="9"/>
-      <c r="D1924" s="2"/>
-    </row>
-    <row r="1925">
-      <c r="A1925" s="11"/>
-      <c r="C1925" s="9"/>
-      <c r="D1925" s="2"/>
-    </row>
-    <row r="1926">
-      <c r="A1926" s="11"/>
-      <c r="C1926" s="9"/>
-      <c r="D1926" s="2"/>
-    </row>
-    <row r="1927">
-      <c r="A1927" s="11"/>
-      <c r="C1927" s="9"/>
-      <c r="D1927" s="2"/>
-    </row>
-    <row r="1928">
-      <c r="A1928" s="11"/>
-      <c r="C1928" s="9"/>
-      <c r="D1928" s="2"/>
-    </row>
-    <row r="1929">
-      <c r="A1929" s="11"/>
-      <c r="C1929" s="9"/>
-      <c r="D1929" s="2"/>
-    </row>
-    <row r="1930">
-      <c r="A1930" s="11"/>
-      <c r="C1930" s="9"/>
-      <c r="D1930" s="2"/>
-    </row>
-    <row r="1931">
-      <c r="A1931" s="11"/>
-      <c r="C1931" s="9"/>
-      <c r="D1931" s="2"/>
-    </row>
-    <row r="1932">
-      <c r="A1932" s="11"/>
-      <c r="C1932" s="9"/>
-      <c r="D1932" s="2"/>
-    </row>
-    <row r="1933">
-      <c r="A1933" s="11"/>
-      <c r="C1933" s="9"/>
-      <c r="D1933" s="2"/>
-    </row>
-    <row r="1934">
-      <c r="A1934" s="11"/>
-      <c r="C1934" s="9"/>
-      <c r="D1934" s="2"/>
-    </row>
-    <row r="1935">
-      <c r="A1935" s="11"/>
-      <c r="C1935" s="9"/>
-      <c r="D1935" s="2"/>
-    </row>
-    <row r="1936">
-      <c r="A1936" s="11"/>
-      <c r="C1936" s="9"/>
-      <c r="D1936" s="2"/>
-    </row>
-    <row r="1937">
-      <c r="A1937" s="11"/>
-      <c r="C1937" s="9"/>
-      <c r="D1937" s="2"/>
-    </row>
-    <row r="1938">
-      <c r="A1938" s="11"/>
-      <c r="C1938" s="9"/>
-      <c r="D1938" s="2"/>
-    </row>
-    <row r="1939">
-      <c r="A1939" s="11"/>
-      <c r="C1939" s="9"/>
-      <c r="D1939" s="2"/>
-    </row>
-    <row r="1940">
-      <c r="A1940" s="11"/>
-      <c r="C1940" s="9"/>
-      <c r="D1940" s="2"/>
-    </row>
-    <row r="1941">
-      <c r="A1941" s="11"/>
-      <c r="C1941" s="9"/>
-      <c r="D1941" s="2"/>
-    </row>
-    <row r="1942">
-      <c r="A1942" s="11"/>
-      <c r="C1942" s="9"/>
-      <c r="D1942" s="2"/>
-    </row>
-    <row r="1943">
-      <c r="A1943" s="11"/>
-      <c r="C1943" s="9"/>
-      <c r="D1943" s="2"/>
-    </row>
-    <row r="1944">
-      <c r="A1944" s="11"/>
-      <c r="C1944" s="9"/>
-      <c r="D1944" s="2"/>
-    </row>
-    <row r="1945">
-      <c r="A1945" s="11"/>
-      <c r="C1945" s="9"/>
-      <c r="D1945" s="2"/>
-    </row>
-    <row r="1946">
-      <c r="A1946" s="11"/>
-      <c r="C1946" s="9"/>
-      <c r="D1946" s="2"/>
-    </row>
-    <row r="1947">
-      <c r="A1947" s="11"/>
-      <c r="C1947" s="9"/>
-      <c r="D1947" s="2"/>
-    </row>
-    <row r="1948">
-      <c r="A1948" s="11"/>
-      <c r="C1948" s="9"/>
-      <c r="D1948" s="2"/>
-    </row>
-    <row r="1949">
-      <c r="A1949" s="11"/>
-      <c r="C1949" s="9"/>
-      <c r="D1949" s="2"/>
-    </row>
-    <row r="1950">
-      <c r="A1950" s="11"/>
-      <c r="C1950" s="9"/>
-      <c r="D1950" s="2"/>
-    </row>
-    <row r="1951">
-      <c r="A1951" s="11"/>
-      <c r="C1951" s="9"/>
-      <c r="D1951" s="2"/>
-    </row>
-    <row r="1952">
-      <c r="A1952" s="11"/>
-      <c r="C1952" s="9"/>
-      <c r="D1952" s="2"/>
-    </row>
-    <row r="1953">
-      <c r="A1953" s="11"/>
-      <c r="C1953" s="9"/>
-      <c r="D1953" s="2"/>
-    </row>
-    <row r="1954">
-      <c r="A1954" s="11"/>
-      <c r="C1954" s="9"/>
-      <c r="D1954" s="2"/>
-    </row>
-    <row r="1955">
-      <c r="A1955" s="11"/>
-      <c r="C1955" s="9"/>
-      <c r="D1955" s="2"/>
-    </row>
-    <row r="1956">
-      <c r="A1956" s="11"/>
-      <c r="C1956" s="9"/>
-      <c r="D1956" s="2"/>
-    </row>
-    <row r="1957">
-      <c r="A1957" s="11"/>
-      <c r="C1957" s="9"/>
-      <c r="D1957" s="2"/>
-    </row>
-    <row r="1958">
-      <c r="A1958" s="11"/>
-      <c r="C1958" s="9"/>
-      <c r="D1958" s="2"/>
-    </row>
-    <row r="1959">
-      <c r="A1959" s="11"/>
-      <c r="C1959" s="9"/>
-      <c r="D1959" s="2"/>
-    </row>
-    <row r="1960">
-      <c r="A1960" s="11"/>
-      <c r="C1960" s="9"/>
-      <c r="D1960" s="2"/>
-    </row>
-    <row r="1961">
-      <c r="A1961" s="11"/>
-      <c r="C1961" s="9"/>
-      <c r="D1961" s="2"/>
-    </row>
-    <row r="1962">
-      <c r="A1962" s="11"/>
-      <c r="C1962" s="9"/>
-      <c r="D1962" s="2"/>
-    </row>
-    <row r="1963">
-      <c r="A1963" s="11"/>
-      <c r="C1963" s="9"/>
-      <c r="D1963" s="2"/>
-    </row>
-    <row r="1964">
-      <c r="A1964" s="11"/>
-      <c r="C1964" s="9"/>
-      <c r="D1964" s="2"/>
-    </row>
-    <row r="1965">
-      <c r="A1965" s="11"/>
-      <c r="C1965" s="9"/>
-      <c r="D1965" s="2"/>
-    </row>
-    <row r="1966">
-      <c r="A1966" s="11"/>
-      <c r="C1966" s="9"/>
-      <c r="D1966" s="2"/>
-    </row>
-    <row r="1967">
-      <c r="A1967" s="11"/>
-      <c r="C1967" s="9"/>
-      <c r="D1967" s="2"/>
-    </row>
-    <row r="1968">
-      <c r="A1968" s="11"/>
-      <c r="C1968" s="9"/>
-      <c r="D1968" s="2"/>
-    </row>
-    <row r="1969">
-      <c r="A1969" s="11"/>
-      <c r="C1969" s="9"/>
-      <c r="D1969" s="2"/>
-    </row>
-    <row r="1970">
-      <c r="A1970" s="11"/>
-      <c r="C1970" s="9"/>
-      <c r="D1970" s="2"/>
-    </row>
-    <row r="1971">
-      <c r="A1971" s="11"/>
-      <c r="C1971" s="9"/>
-      <c r="D1971" s="2"/>
-    </row>
-    <row r="1972">
-      <c r="A1972" s="11"/>
-      <c r="C1972" s="9"/>
-      <c r="D1972" s="2"/>
-    </row>
-    <row r="1973">
-      <c r="A1973" s="11"/>
-      <c r="C1973" s="9"/>
-      <c r="D1973" s="2"/>
-    </row>
-    <row r="1974">
-      <c r="A1974" s="11"/>
-      <c r="C1974" s="9"/>
-      <c r="D1974" s="2"/>
-    </row>
-    <row r="1975">
-      <c r="A1975" s="11"/>
-      <c r="C1975" s="9"/>
-      <c r="D1975" s="2"/>
-    </row>
-    <row r="1976">
-      <c r="A1976" s="11"/>
-      <c r="C1976" s="9"/>
-      <c r="D1976" s="2"/>
-    </row>
-    <row r="1977">
-      <c r="A1977" s="11"/>
-      <c r="C1977" s="9"/>
-      <c r="D1977" s="2"/>
-    </row>
-    <row r="1978">
-      <c r="A1978" s="11"/>
-      <c r="C1978" s="9"/>
-      <c r="D1978" s="2"/>
-    </row>
-    <row r="1979">
-      <c r="A1979" s="11"/>
-      <c r="C1979" s="9"/>
-      <c r="D1979" s="2"/>
-    </row>
-    <row r="1980">
-      <c r="A1980" s="11"/>
-      <c r="C1980" s="9"/>
-      <c r="D1980" s="2"/>
-    </row>
-    <row r="1981">
-      <c r="A1981" s="11"/>
-      <c r="C1981" s="9"/>
-      <c r="D1981" s="2"/>
-    </row>
-    <row r="1982">
-      <c r="A1982" s="11"/>
-      <c r="C1982" s="9"/>
-      <c r="D1982" s="2"/>
-    </row>
-    <row r="1983">
-      <c r="A1983" s="11"/>
-      <c r="C1983" s="9"/>
-      <c r="D1983" s="2"/>
-    </row>
-    <row r="1984">
-      <c r="A1984" s="11"/>
-      <c r="C1984" s="9"/>
-      <c r="D1984" s="2"/>
-    </row>
-    <row r="1985">
-      <c r="A1985" s="11"/>
-      <c r="C1985" s="9"/>
-      <c r="D1985" s="2"/>
-    </row>
-    <row r="1986">
-      <c r="A1986" s="11"/>
-      <c r="C1986" s="9"/>
-      <c r="D1986" s="2"/>
-    </row>
-    <row r="1987">
-      <c r="A1987" s="11"/>
-      <c r="C1987" s="9"/>
-      <c r="D1987" s="2"/>
-    </row>
-    <row r="1988">
-      <c r="A1988" s="11"/>
-      <c r="C1988" s="9"/>
-      <c r="D1988" s="2"/>
-    </row>
-    <row r="1989">
-      <c r="A1989" s="11"/>
-      <c r="C1989" s="9"/>
-      <c r="D1989" s="2"/>
-    </row>
-    <row r="1990">
-      <c r="A1990" s="11"/>
-      <c r="C1990" s="9"/>
-      <c r="D1990" s="2"/>
-    </row>
-    <row r="1991">
-      <c r="A1991" s="11"/>
-      <c r="C1991" s="9"/>
-      <c r="D1991" s="2"/>
-    </row>
-    <row r="1992">
-      <c r="A1992" s="11"/>
-      <c r="C1992" s="9"/>
-      <c r="D1992" s="2"/>
-    </row>
-    <row r="1993">
-      <c r="A1993" s="11"/>
-      <c r="C1993" s="9"/>
-      <c r="D1993" s="2"/>
-    </row>
-    <row r="1994">
-      <c r="A1994" s="11"/>
-      <c r="C1994" s="9"/>
-      <c r="D1994" s="2"/>
-    </row>
-    <row r="1995">
-      <c r="A1995" s="11"/>
-      <c r="C1995" s="9"/>
-      <c r="D1995" s="2"/>
-    </row>
-    <row r="1996">
-      <c r="A1996" s="11"/>
-      <c r="C1996" s="9"/>
-      <c r="D1996" s="2"/>
-    </row>
-    <row r="1997">
-      <c r="A1997" s="11"/>
-      <c r="C1997" s="9"/>
-      <c r="D1997" s="2"/>
-    </row>
-    <row r="1998">
-      <c r="A1998" s="11"/>
-      <c r="C1998" s="9"/>
-      <c r="D1998" s="2"/>
-    </row>
-    <row r="1999">
-      <c r="A1999" s="11"/>
-      <c r="C1999" s="9"/>
-      <c r="D1999" s="2"/>
-    </row>
-    <row r="2000">
-      <c r="A2000" s="11"/>
-      <c r="C2000" s="9"/>
-      <c r="D2000" s="2"/>
-    </row>
-    <row r="2001">
-      <c r="A2001" s="11"/>
-      <c r="C2001" s="9"/>
-      <c r="D2001" s="2"/>
-    </row>
-    <row r="2002">
-      <c r="A2002" s="11"/>
-      <c r="C2002" s="9"/>
-      <c r="D2002" s="2"/>
-    </row>
-    <row r="2003">
-      <c r="A2003" s="11"/>
-      <c r="C2003" s="9"/>
-      <c r="D2003" s="2"/>
-    </row>
-    <row r="2004">
-      <c r="A2004" s="11"/>
-      <c r="C2004" s="9"/>
-      <c r="D2004" s="2"/>
-    </row>
-    <row r="2005">
-      <c r="A2005" s="11"/>
-      <c r="C2005" s="9"/>
-      <c r="D2005" s="2"/>
-    </row>
-    <row r="2006">
-      <c r="A2006" s="11"/>
-      <c r="C2006" s="9"/>
-      <c r="D2006" s="2"/>
-    </row>
-    <row r="2007">
-      <c r="A2007" s="11"/>
-      <c r="C2007" s="9"/>
-      <c r="D2007" s="2"/>
-    </row>
-    <row r="2008">
-      <c r="A2008" s="11"/>
-      <c r="C2008" s="9"/>
-      <c r="D2008" s="2"/>
-    </row>
-    <row r="2009">
-      <c r="A2009" s="11"/>
-      <c r="C2009" s="9"/>
-      <c r="D2009" s="2"/>
-    </row>
-    <row r="2010">
-      <c r="A2010" s="11"/>
-      <c r="C2010" s="9"/>
-      <c r="D2010" s="2"/>
-    </row>
-    <row r="2011">
-      <c r="A2011" s="11"/>
-      <c r="C2011" s="9"/>
-      <c r="D2011" s="2"/>
-    </row>
-    <row r="2012">
-      <c r="A2012" s="11"/>
-      <c r="C2012" s="9"/>
-      <c r="D2012" s="2"/>
-    </row>
-    <row r="2013">
-      <c r="A2013" s="11"/>
-      <c r="C2013" s="9"/>
-      <c r="D2013" s="2"/>
-    </row>
-    <row r="2014">
-      <c r="A2014" s="11"/>
-      <c r="C2014" s="9"/>
-      <c r="D2014" s="2"/>
-    </row>
-    <row r="2015">
-      <c r="A2015" s="11"/>
-      <c r="C2015" s="9"/>
-      <c r="D2015" s="2"/>
-    </row>
-    <row r="2016">
-      <c r="A2016" s="11"/>
-      <c r="C2016" s="9"/>
-      <c r="D2016" s="2"/>
-    </row>
-    <row r="2017">
-      <c r="A2017" s="11"/>
-      <c r="C2017" s="9"/>
-      <c r="D2017" s="2"/>
-    </row>
-    <row r="2018">
-      <c r="A2018" s="11"/>
-      <c r="C2018" s="9"/>
-      <c r="D2018" s="2"/>
-    </row>
-    <row r="2019">
-      <c r="A2019" s="11"/>
-      <c r="C2019" s="9"/>
-      <c r="D2019" s="2"/>
-    </row>
-    <row r="2020">
-      <c r="A2020" s="11"/>
-      <c r="C2020" s="9"/>
-      <c r="D2020" s="2"/>
-    </row>
-    <row r="2021">
-      <c r="A2021" s="11"/>
-      <c r="C2021" s="9"/>
-      <c r="D2021" s="2"/>
-    </row>
-    <row r="2022">
-      <c r="A2022" s="11"/>
-      <c r="C2022" s="9"/>
-      <c r="D2022" s="2"/>
-    </row>
-    <row r="2023">
-      <c r="A2023" s="11"/>
-      <c r="C2023" s="9"/>
-      <c r="D2023" s="2"/>
-    </row>
-    <row r="2024">
-      <c r="A2024" s="11"/>
-      <c r="C2024" s="9"/>
-      <c r="D2024" s="2"/>
-    </row>
-    <row r="2025">
-      <c r="A2025" s="11"/>
-      <c r="C2025" s="9"/>
-      <c r="D2025" s="2"/>
-    </row>
-    <row r="2026">
-      <c r="A2026" s="11"/>
-      <c r="C2026" s="9"/>
-      <c r="D2026" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A933"/>

</xml_diff>

<commit_message>
add pnplacehold test (#79)
</commit_message>
<xml_diff>
--- a/csv/merge.xlsx
+++ b/csv/merge.xlsx
@@ -6157,7 +6157,7 @@
 &lt;select_end&gt;&lt;break&gt;</t>
   </si>
   <si>
-    <t>Hello! Good to see you again!
+    <t>Hello! Good to see you, &lt;pnplacehold&gt;!
 Do you have something to report?
 &lt;select_se_off&gt;
 Report
@@ -6184,7 +6184,7 @@
 &lt;select_end&gt;&lt;break&gt;</t>
   </si>
   <si>
-    <t>Hello! Nice work!
+    <t>Hello! Nice work, &lt;pnplacehold&gt;!
 Do you have something to report?
 &lt;select_se_off&gt;
 Report
@@ -6208,7 +6208,7 @@
 &lt;select_end&gt;&lt;break&gt;</t>
   </si>
   <si>
-    <t>Well, look who it is!
+    <t>Well, if it isn't &lt;pnplacehold&gt;!
 Do you have something to report?
 &lt;select_se_off&gt;
 Report
@@ -19500,7 +19500,7 @@
   <si>
     <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;...I too watched your battle. I was
 terrified of his beastly form, which he had
-gained from the source of darkness.&lt;bw_break&gt;</t>
+gained from the Source of Darkness.&lt;bw_break&gt;</t>
   </si>
   <si>
     <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;「ですが　あなたは　恐れなかった。
@@ -19510,7 +19510,7 @@
   <si>
     <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;But you showed no fear. It was at that
 moment I knew you were worthy of being a
-hero.</t>
+champion.</t>
   </si>
   <si>
     <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;「その確信は　まちがいではなかった。
@@ -19647,7 +19647,7 @@
 　アンルシア姫を救いだしたと　聞いています。&lt;bw_break&gt;</t>
   </si>
   <si>
-    <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;You met that hero in the false world,
+    <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;You met him in the false world,
 and together you rescued Anlucia, who was at
 the time just a simple village girl.&lt;bw_break&gt;</t>
   </si>
@@ -19673,7 +19673,7 @@
   </si>
   <si>
     <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;It was also quite unexpected that the same
-hero would later appear in our world and
+character would later appear in our world and
 have an important role to play.&lt;bw_break&gt;</t>
   </si>
   <si>
@@ -19694,7 +19694,7 @@
   <si>
     <t>&lt;attr&gt;&lt;feel_custom&gt;&lt;end_attr&gt;If he were not a character from a story,
 then he could've had the potential to be
-invited to Fourion as a hero.&lt;bw_break&gt;</t>
+invited to Fourion as a champion.&lt;bw_break&gt;</t>
   </si>
   <si>
     <t>「いたましい事故で　多くの命が失われた
@@ -24991,8 +24991,7 @@
 BUT THIS...MIGHT BE THE...&lt;se_nots S3_DWF5_001 001&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">
-「ワタシノ体内ニアル　太陽ノ弾ハ……
+    <t>「ワタシノ体内ニアル　太陽ノ弾ハ……
 　リウ老師ガ　生涯ヲカケ……作リ上ゲタ……
 　大魔神ヘノ……タッタヒトツノ　対抗策……。
 &lt;br&gt;

</xml_diff>